<commit_message>
Testing probabilistic batch normalization.
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\phd_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13EA86A4-D12A-4D1B-B96F-2F3F02764CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCE75EB-2F8F-458F-87C1-F30BC5EE4C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FFBB5989-5F03-4E6C-92F7-2FA7EA34683B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2858" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2881" uniqueCount="488">
   <si>
     <t>ToDo</t>
   </si>
@@ -1501,6 +1501,12 @@
   </si>
   <si>
     <t>26.04.2022</t>
+  </si>
+  <si>
+    <t>27.04.2022</t>
+  </si>
+  <si>
+    <t>Phd: Implement discrete Bayesian Optimization</t>
   </si>
 </sst>
 </file>
@@ -4005,10 +4011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6010993A-D4ED-4EB4-B776-F18BCFD807DB}">
-  <dimension ref="A1:G2558"/>
+  <dimension ref="A1:G2580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2533" workbookViewId="0">
-      <selection activeCell="D2555" sqref="D2555"/>
+    <sheetView tabSelected="1" topLeftCell="B2559" workbookViewId="0">
+      <selection activeCell="D2574" sqref="D2574"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33855,7 +33861,7 @@
         <v>10</v>
       </c>
       <c r="C2551" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D2551" s="1"/>
     </row>
@@ -33938,8 +33944,272 @@
       </c>
       <c r="C2558" s="7">
         <f>SUM(C2539:C2557)</f>
-        <v>1</v>
-      </c>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2559" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2559" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="B2559" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2559" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2559" s="4"/>
+    </row>
+    <row r="2560" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2560" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B2560" s="7">
+        <v>8</v>
+      </c>
+      <c r="C2560" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2560" s="11"/>
+    </row>
+    <row r="2561" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2561" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="B2561" s="7">
+        <v>24</v>
+      </c>
+      <c r="C2561" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2561" s="7"/>
+    </row>
+    <row r="2562" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2562" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="B2562" s="7">
+        <v>12</v>
+      </c>
+      <c r="C2562" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2562" s="7"/>
+    </row>
+    <row r="2563" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2563" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="B2563" s="7">
+        <v>12</v>
+      </c>
+      <c r="C2563" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2563" s="1"/>
+    </row>
+    <row r="2564" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2564" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="B2564" s="7">
+        <v>6</v>
+      </c>
+      <c r="C2564" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2564" s="7"/>
+    </row>
+    <row r="2565" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2565" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B2565" s="1">
+        <v>8</v>
+      </c>
+      <c r="C2565" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2565" s="1"/>
+    </row>
+    <row r="2566" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2566" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="B2566" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2566" s="7">
+        <v>2</v>
+      </c>
+      <c r="D2566" s="1"/>
+    </row>
+    <row r="2567" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2567" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B2567" s="7">
+        <v>6</v>
+      </c>
+      <c r="C2567" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2567" s="1"/>
+    </row>
+    <row r="2568" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2568" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2568" s="7">
+        <v>12</v>
+      </c>
+      <c r="C2568" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2568" s="7"/>
+    </row>
+    <row r="2569" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2569" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="B2569" s="7">
+        <v>12</v>
+      </c>
+      <c r="C2569" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2569" s="7"/>
+    </row>
+    <row r="2570" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2570" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B2570" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2570" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2570" s="1"/>
+    </row>
+    <row r="2571" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2571" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B2571" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2571" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2571" s="1"/>
+    </row>
+    <row r="2572" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2572" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B2572" s="1">
+        <v>10</v>
+      </c>
+      <c r="C2572" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2572" s="1"/>
+    </row>
+    <row r="2573" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2573" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="B2573" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2573" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2573" s="7"/>
+    </row>
+    <row r="2574" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2574" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B2574" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2574" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2574" s="1"/>
+    </row>
+    <row r="2575" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2575" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="B2575" s="7">
+        <v>6</v>
+      </c>
+      <c r="C2575" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2575" s="1"/>
+    </row>
+    <row r="2576" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2576" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B2576" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2576" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2576" s="1"/>
+    </row>
+    <row r="2577" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2577" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="B2577" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2577" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2577" s="1"/>
+    </row>
+    <row r="2578" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2578" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B2578" s="1">
+        <v>8</v>
+      </c>
+      <c r="C2578" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2578" s="1"/>
+    </row>
+    <row r="2579" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2579" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="B2579" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2579" s="7">
+        <v>2</v>
+      </c>
+      <c r="D2579" s="1"/>
+    </row>
+    <row r="2580" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2580" s="1"/>
+      <c r="B2580" s="1">
+        <f>SUM(B2560:B2579)</f>
+        <v>153</v>
+      </c>
+      <c r="C2580" s="7">
+        <f>SUM(C2560:C2579)</f>
+        <v>4</v>
+      </c>
+      <c r="D2580" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35343,39 +35613,48 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63AE077A-6D37-41FE-B854-DE1F0AAE9930}">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="28">
         <v>0.92519999742507897</v>
       </c>
       <c r="B1" s="28">
         <v>0.68922623762082602</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G1">
+        <v>0.92483000159263595</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="28">
         <v>0.92518000602722195</v>
       </c>
       <c r="B2" s="28">
         <v>0.75944833021171398</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>0.92431000471115099</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="28">
         <v>0.92517000436782804</v>
       </c>
       <c r="B3" s="28">
         <v>0.70375937279584999</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>0.92413998842239398</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
         <v>0.92486999630928002</v>
       </c>
@@ -35386,136 +35665,187 @@
         <f>CORREL(A1:A99,B1:B99)</f>
         <v>0.30280612852118793</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>0.92348001003265401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
         <v>0.92418999671935997</v>
       </c>
       <c r="B5" s="28">
         <v>0.122700715408658</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>0.92332999706268304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="28">
         <v>0.92404999732971205</v>
       </c>
       <c r="B6" s="28">
         <v>0.39328405962294199</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>0.92307000160217301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="28">
         <v>0.92292000055313095</v>
       </c>
       <c r="B7" s="28">
         <v>0.93172544467337703</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>0.92292000055313095</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="28">
         <v>0.92286999821662896</v>
       </c>
       <c r="B8" s="28">
         <v>0.357795993118804</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>0.92289999723434402</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="28">
         <v>0.92277999520301801</v>
       </c>
       <c r="B9" s="28">
         <v>0.62195093022721604</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>0.92282000184059099</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="28">
         <v>0.92255999445915204</v>
       </c>
       <c r="B10" s="28">
         <v>0.29109230601219099</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>0.92268000245094295</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
         <v>0.92237000465393104</v>
       </c>
       <c r="B11" s="28">
         <v>0.55801829041753304</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>0.92245000004768396</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="28">
         <v>0.92228000164031998</v>
       </c>
       <c r="B12" s="28">
         <v>7.1187612213445203E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>0.92234000563621499</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="28">
         <v>0.92226001024246196</v>
       </c>
       <c r="B13" s="28">
         <v>0.415237510565102</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>0.92222999334335298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="28">
         <v>0.92218999266624502</v>
       </c>
       <c r="B14" s="28">
         <v>0.75820255770711797</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>0.92195000648498504</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="28">
         <v>0.92217000722885101</v>
       </c>
       <c r="B15" s="28">
         <v>0.55244033312234897</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <v>0.921819996833801</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="28">
         <v>0.92212999463081402</v>
       </c>
       <c r="B16" s="28">
         <v>0.44051171617859503</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>0.92170000076293901</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
         <v>0.92207998633384702</v>
       </c>
       <c r="B17" s="28">
         <v>0.60406765669463403</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>0.92139999270439099</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="28">
         <v>0.92203000783920297</v>
       </c>
       <c r="B18" s="28">
         <v>0.94301731645230302</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>0.92057999372482302</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="28">
         <v>0.92203000187873796</v>
       </c>
       <c r="B19" s="28">
         <v>0.21229149824246801</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>0.92008000016212499</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="28">
         <v>0.92200999259948702</v>
       </c>
       <c r="B20" s="28">
         <v>0.20426367129478301</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>0.91931000947952302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="28">
         <v>0.92199000120162999</v>
       </c>
@@ -35523,7 +35853,7 @@
         <v>0.50884061267337899</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="28">
         <v>0.92197000384330796</v>
       </c>
@@ -35531,7 +35861,7 @@
         <v>0.38931491911738397</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="28">
         <v>0.92183000445365904</v>
       </c>
@@ -35539,7 +35869,7 @@
         <v>0.28973208632376202</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="28">
         <v>0.92178000807762095</v>
       </c>
@@ -35547,7 +35877,7 @@
         <v>0.90858184975631295</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="28">
         <v>0.92177000045776403</v>
       </c>
@@ -35555,7 +35885,7 @@
         <v>0.86336904770637701</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="28">
         <v>0.92171999812126204</v>
       </c>
@@ -35563,7 +35893,7 @@
         <v>0.97772281529024696</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="28">
         <v>0.92168999910354599</v>
       </c>
@@ -35571,7 +35901,7 @@
         <v>0.41485442547883999</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="28">
         <v>0.92168999910354599</v>
       </c>
@@ -35579,7 +35909,7 @@
         <v>0.94643173274833503</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="28">
         <v>0.92165000438690203</v>
       </c>
@@ -35587,7 +35917,7 @@
         <v>0.47027263767153998</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="28">
         <v>0.92153000831604004</v>
       </c>
@@ -35595,7 +35925,7 @@
         <v>0.42956380818251599</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="28">
         <v>0.92153000235557603</v>
       </c>
@@ -35603,7 +35933,7 @@
         <v>0.87123484986671695</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="28">
         <v>0.92148000597953805</v>
       </c>

</xml_diff>

<commit_message>
Probabilistic Batch Normalization Tests have been succesful.
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\phd_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7700B1CA-4892-4441-800B-BB9DDF23D0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACE99B6-9458-4F47-8CA3-483118E0FC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FFBB5989-5F03-4E6C-92F7-2FA7EA34683B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2929" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2977" uniqueCount="498">
   <si>
     <t>ToDo</t>
   </si>
@@ -1522,6 +1522,21 @@
   </si>
   <si>
     <t>Phd: Write Fashion MNIST Experiments</t>
+  </si>
+  <si>
+    <t>Phd-Blackshark: Docker tutorial</t>
+  </si>
+  <si>
+    <t>30.04.2022</t>
+  </si>
+  <si>
+    <t>1.05.2022</t>
+  </si>
+  <si>
+    <t>Insumo: Select Mixpanel categories</t>
+  </si>
+  <si>
+    <t>Phd: Run 3 blocks experiment in Home computer</t>
   </si>
 </sst>
 </file>
@@ -4026,10 +4041,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6010993A-D4ED-4EB4-B776-F18BCFD807DB}">
-  <dimension ref="A1:G2626"/>
+  <dimension ref="A1:G2673"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2602" workbookViewId="0">
-      <selection activeCell="A2613" sqref="A2613"/>
+    <sheetView tabSelected="1" topLeftCell="A2650" workbookViewId="0">
+      <selection activeCell="D2659" sqref="D2659"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34570,7 +34585,7 @@
         <v>6</v>
       </c>
       <c r="C2609" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2609" s="7"/>
     </row>
@@ -34660,7 +34675,7 @@
     </row>
     <row r="2617" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2617" s="1" t="s">
-        <v>466</v>
+        <v>493</v>
       </c>
       <c r="B2617" s="1">
         <v>10</v>
@@ -34690,7 +34705,7 @@
         <v>3</v>
       </c>
       <c r="C2619" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D2619" s="1"/>
     </row>
@@ -34738,7 +34753,7 @@
         <v>8</v>
       </c>
       <c r="C2623" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2623" s="1"/>
     </row>
@@ -34768,9 +34783,565 @@
       </c>
       <c r="C2626" s="7">
         <f>SUM(C2605:C2624)</f>
+        <v>10</v>
+      </c>
+      <c r="D2626" s="1"/>
+    </row>
+    <row r="2627" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2627" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="B2627" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2627" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2627" s="4"/>
+    </row>
+    <row r="2628" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2628" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B2628" s="7">
+        <v>8</v>
+      </c>
+      <c r="C2628" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2628" s="11"/>
+    </row>
+    <row r="2629" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2629" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="B2629" s="7">
+        <v>24</v>
+      </c>
+      <c r="C2629" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2629" s="7"/>
+    </row>
+    <row r="2630" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2630" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="B2630" s="7">
+        <v>12</v>
+      </c>
+      <c r="C2630" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2630" s="7"/>
+    </row>
+    <row r="2631" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2631" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="B2631" s="7">
+        <v>12</v>
+      </c>
+      <c r="C2631" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2631" s="1"/>
+    </row>
+    <row r="2632" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2632" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="B2632" s="7">
+        <v>6</v>
+      </c>
+      <c r="C2632" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2632" s="7"/>
+    </row>
+    <row r="2633" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2633" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B2633" s="1">
+        <v>8</v>
+      </c>
+      <c r="C2633" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2633" s="1"/>
+    </row>
+    <row r="2634" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2634" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="B2634" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2634" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2634" s="1"/>
+    </row>
+    <row r="2635" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2635" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B2635" s="7">
+        <v>6</v>
+      </c>
+      <c r="C2635" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2635" s="1"/>
+    </row>
+    <row r="2636" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2636" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2636" s="7">
+        <v>24</v>
+      </c>
+      <c r="C2636" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2636" s="7"/>
+    </row>
+    <row r="2637" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2637" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="B2637" s="7">
+        <v>12</v>
+      </c>
+      <c r="C2637" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2637" s="7"/>
+    </row>
+    <row r="2638" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2638" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B2638" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2638" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2638" s="1"/>
+    </row>
+    <row r="2639" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2639" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B2639" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2639" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2639" s="1"/>
+    </row>
+    <row r="2640" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2640" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B2640" s="1">
+        <v>10</v>
+      </c>
+      <c r="C2640" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2640" s="1"/>
+    </row>
+    <row r="2641" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2641" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="B2641" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2641" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2641" s="7"/>
+    </row>
+    <row r="2642" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2642" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B2642" s="1">
         <v>3</v>
       </c>
-      <c r="D2626" s="1"/>
+      <c r="C2642" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2642" s="1"/>
+    </row>
+    <row r="2643" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2643" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="B2643" s="7">
+        <v>6</v>
+      </c>
+      <c r="C2643" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2643" s="1"/>
+    </row>
+    <row r="2644" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2644" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B2644" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2644" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2644" s="1"/>
+    </row>
+    <row r="2645" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2645" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="B2645" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2645" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2645" s="1"/>
+    </row>
+    <row r="2646" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2646" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B2646" s="1">
+        <v>8</v>
+      </c>
+      <c r="C2646" s="7">
+        <v>8</v>
+      </c>
+      <c r="D2646" s="1"/>
+    </row>
+    <row r="2647" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2647" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B2647" s="1">
+        <v>24</v>
+      </c>
+      <c r="C2647" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2647" s="1"/>
+    </row>
+    <row r="2648" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2648" s="1"/>
+      <c r="B2648" s="1"/>
+      <c r="C2648" s="1"/>
+      <c r="D2648" s="1"/>
+    </row>
+    <row r="2649" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2649" s="1"/>
+      <c r="B2649" s="1">
+        <f>SUM(B2628:B2647)</f>
+        <v>187</v>
+      </c>
+      <c r="C2649" s="7">
+        <f>SUM(C2628:C2647)</f>
+        <v>8</v>
+      </c>
+      <c r="D2649" s="1"/>
+    </row>
+    <row r="2650" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2650" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="B2650" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2650" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2650" s="4"/>
+    </row>
+    <row r="2651" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2651" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B2651" s="7">
+        <v>8</v>
+      </c>
+      <c r="C2651" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2651" s="11"/>
+    </row>
+    <row r="2652" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2652" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="B2652" s="7">
+        <v>24</v>
+      </c>
+      <c r="C2652" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2652" s="7"/>
+    </row>
+    <row r="2653" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2653" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="B2653" s="7">
+        <v>12</v>
+      </c>
+      <c r="C2653" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2653" s="7"/>
+    </row>
+    <row r="2654" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2654" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="B2654" s="7">
+        <v>12</v>
+      </c>
+      <c r="C2654" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2654" s="1"/>
+    </row>
+    <row r="2655" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2655" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="B2655" s="7">
+        <v>6</v>
+      </c>
+      <c r="C2655" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2655" s="7"/>
+    </row>
+    <row r="2656" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2656" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B2656" s="1">
+        <v>8</v>
+      </c>
+      <c r="C2656" s="7">
+        <v>3</v>
+      </c>
+      <c r="D2656" s="1"/>
+    </row>
+    <row r="2657" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2657" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="B2657" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2657" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2657" s="1"/>
+    </row>
+    <row r="2658" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2658" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B2658" s="7">
+        <v>6</v>
+      </c>
+      <c r="C2658" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2658" s="1"/>
+    </row>
+    <row r="2659" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2659" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2659" s="7">
+        <v>24</v>
+      </c>
+      <c r="C2659" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2659" s="7"/>
+    </row>
+    <row r="2660" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2660" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="B2660" s="7">
+        <v>12</v>
+      </c>
+      <c r="C2660" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2660" s="7"/>
+    </row>
+    <row r="2661" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2661" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B2661" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2661" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2661" s="1"/>
+    </row>
+    <row r="2662" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2662" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B2662" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2662" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2662" s="1"/>
+    </row>
+    <row r="2663" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2663" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B2663" s="1">
+        <v>10</v>
+      </c>
+      <c r="C2663" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2663" s="1"/>
+    </row>
+    <row r="2664" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2664" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="B2664" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2664" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2664" s="7"/>
+    </row>
+    <row r="2665" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2665" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B2665" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2665" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2665" s="1"/>
+    </row>
+    <row r="2666" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2666" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="B2666" s="7">
+        <v>6</v>
+      </c>
+      <c r="C2666" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2666" s="1"/>
+    </row>
+    <row r="2667" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2667" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B2667" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2667" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2667" s="1"/>
+    </row>
+    <row r="2668" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2668" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="B2668" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2668" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2668" s="1"/>
+    </row>
+    <row r="2669" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2669" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B2669" s="1">
+        <v>8</v>
+      </c>
+      <c r="C2669" s="7">
+        <v>8</v>
+      </c>
+      <c r="D2669" s="1"/>
+    </row>
+    <row r="2670" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2670" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B2670" s="1">
+        <v>24</v>
+      </c>
+      <c r="C2670" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2670" s="1"/>
+    </row>
+    <row r="2671" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2671" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B2671" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2671" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2671" s="1"/>
+    </row>
+    <row r="2672" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2672" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B2672" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2672" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2672" s="1"/>
+    </row>
+    <row r="2673" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2673" s="1">
+        <f>SUM(B2651:B2672)</f>
+        <v>194</v>
+      </c>
+      <c r="C2673" s="7">
+        <f>SUM(C2651:C2672)</f>
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
3 Blocks Lenet training.
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\phd_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACE99B6-9458-4F47-8CA3-483118E0FC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE0471F-4BBD-4124-9B97-BCD9AC2189BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FFBB5989-5F03-4E6C-92F7-2FA7EA34683B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2977" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3000" uniqueCount="501">
   <si>
     <t>ToDo</t>
   </si>
@@ -1537,6 +1537,15 @@
   </si>
   <si>
     <t>Phd: Run 3 blocks experiment in Home computer</t>
+  </si>
+  <si>
+    <t>2.05.2022</t>
+  </si>
+  <si>
+    <t>Phd: Test if masking layer works correctly for Gumbel-Softmax routing</t>
+  </si>
+  <si>
+    <t>Phd: Test if averaging layer works correctly for Gumbel-Softmax routing</t>
   </si>
 </sst>
 </file>
@@ -4041,10 +4050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6010993A-D4ED-4EB4-B776-F18BCFD807DB}">
-  <dimension ref="A1:G2673"/>
+  <dimension ref="A1:G2697"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2650" workbookViewId="0">
-      <selection activeCell="D2659" sqref="D2659"/>
+    <sheetView tabSelected="1" topLeftCell="A2672" workbookViewId="0">
+      <selection activeCell="A2694" sqref="A2694:D2694"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35130,14 +35139,14 @@
       <c r="D2655" s="7"/>
     </row>
     <row r="2656" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2656" s="1" t="s">
+      <c r="A2656" s="6" t="s">
         <v>480</v>
       </c>
-      <c r="B2656" s="1">
+      <c r="B2656" s="6">
         <v>8</v>
       </c>
-      <c r="C2656" s="7">
-        <v>3</v>
+      <c r="C2656" s="6">
+        <v>6</v>
       </c>
       <c r="D2656" s="1"/>
     </row>
@@ -35257,7 +35266,7 @@
         <v>6</v>
       </c>
       <c r="C2666" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2666" s="1"/>
     </row>
@@ -35286,16 +35295,16 @@
       <c r="D2668" s="1"/>
     </row>
     <row r="2669" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2669" s="1" t="s">
+      <c r="A2669" s="6" t="s">
         <v>482</v>
       </c>
-      <c r="B2669" s="1">
+      <c r="B2669" s="6">
         <v>8</v>
       </c>
-      <c r="C2669" s="7">
-        <v>8</v>
-      </c>
-      <c r="D2669" s="1"/>
+      <c r="C2669" s="6">
+        <v>9</v>
+      </c>
+      <c r="D2669" s="6"/>
     </row>
     <row r="2670" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2670" s="1" t="s">
@@ -35310,13 +35319,13 @@
       <c r="D2670" s="1"/>
     </row>
     <row r="2671" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2671" s="1" t="s">
+      <c r="A2671" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="B2671" s="1">
-        <v>4</v>
-      </c>
-      <c r="C2671" s="1">
+      <c r="B2671" s="6">
+        <v>4</v>
+      </c>
+      <c r="C2671" s="6">
         <v>0</v>
       </c>
       <c r="D2671" s="1"/>
@@ -35333,15 +35342,291 @@
       </c>
       <c r="D2672" s="1"/>
     </row>
-    <row r="2673" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2673" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2673" s="1">
         <f>SUM(B2651:B2672)</f>
         <v>194</v>
       </c>
       <c r="C2673" s="7">
         <f>SUM(C2651:C2672)</f>
-        <v>11</v>
-      </c>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2674" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2674" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="B2674" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2674" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2674" s="4"/>
+    </row>
+    <row r="2675" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2675" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B2675" s="7">
+        <v>8</v>
+      </c>
+      <c r="C2675" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2675" s="11"/>
+    </row>
+    <row r="2676" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2676" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="B2676" s="7">
+        <v>24</v>
+      </c>
+      <c r="C2676" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2676" s="7"/>
+    </row>
+    <row r="2677" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2677" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="B2677" s="7">
+        <v>12</v>
+      </c>
+      <c r="C2677" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2677" s="7"/>
+    </row>
+    <row r="2678" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2678" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="B2678" s="7">
+        <v>12</v>
+      </c>
+      <c r="C2678" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2678" s="7"/>
+    </row>
+    <row r="2679" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2679" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="B2679" s="7">
+        <v>6</v>
+      </c>
+      <c r="C2679" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2679" s="7"/>
+    </row>
+    <row r="2680" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2680" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="B2680" s="7">
+        <v>4</v>
+      </c>
+      <c r="C2680" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2680" s="7"/>
+    </row>
+    <row r="2681" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2681" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="B2681" s="7">
+        <v>6</v>
+      </c>
+      <c r="C2681" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2681" s="7"/>
+    </row>
+    <row r="2682" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2682" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2682" s="7">
+        <v>24</v>
+      </c>
+      <c r="C2682" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2682" s="7"/>
+    </row>
+    <row r="2683" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2683" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="B2683" s="7">
+        <v>12</v>
+      </c>
+      <c r="C2683" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2683" s="7"/>
+    </row>
+    <row r="2684" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2684" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="B2684" s="7">
+        <v>4</v>
+      </c>
+      <c r="C2684" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2684" s="7"/>
+    </row>
+    <row r="2685" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2685" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="B2685" s="7">
+        <v>6</v>
+      </c>
+      <c r="C2685" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2685" s="7"/>
+    </row>
+    <row r="2686" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2686" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="B2686" s="7">
+        <v>10</v>
+      </c>
+      <c r="C2686" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2686" s="7"/>
+    </row>
+    <row r="2687" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2687" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="B2687" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2687" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2687" s="7"/>
+    </row>
+    <row r="2688" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2688" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="B2688" s="7">
+        <v>3</v>
+      </c>
+      <c r="C2688" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2688" s="7"/>
+    </row>
+    <row r="2689" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2689" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="B2689" s="6">
+        <v>4</v>
+      </c>
+      <c r="C2689" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2689" s="6"/>
+    </row>
+    <row r="2690" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2690" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="B2690" s="7">
+        <v>3</v>
+      </c>
+      <c r="C2690" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2690" s="7"/>
+    </row>
+    <row r="2691" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2691" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="B2691" s="7">
+        <v>6</v>
+      </c>
+      <c r="C2691" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2691" s="7"/>
+    </row>
+    <row r="2692" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2692" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="B2692" s="7">
+        <v>24</v>
+      </c>
+      <c r="C2692" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2692" s="7"/>
+    </row>
+    <row r="2693" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2693" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="B2693" s="7">
+        <v>3</v>
+      </c>
+      <c r="C2693" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2693" s="7"/>
+    </row>
+    <row r="2694" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2694" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="B2694" s="6">
+        <v>4</v>
+      </c>
+      <c r="C2694" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2694" s="6"/>
+    </row>
+    <row r="2695" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2695" s="7"/>
+      <c r="B2695" s="7"/>
+      <c r="C2695" s="7"/>
+      <c r="D2695" s="7"/>
+    </row>
+    <row r="2696" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2696" s="7"/>
+      <c r="B2696" s="7"/>
+      <c r="C2696" s="7"/>
+      <c r="D2696" s="7"/>
+    </row>
+    <row r="2697" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2697" s="1"/>
+      <c r="B2697" s="1">
+        <f>SUM(B2675:B2695)</f>
+        <v>176</v>
+      </c>
+      <c r="C2697" s="7">
+        <f>SUM(C2675:C2695)</f>
+        <v>2</v>
+      </c>
+      <c r="D2697" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Gumbel Softmax First Experiments
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\phd_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C6B543-2F0E-445D-9869-8328F696D616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00F0B5D-0019-433E-B216-08F37554DF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3259" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3300" uniqueCount="552">
   <si>
     <t>ToDo</t>
   </si>
@@ -1692,6 +1692,15 @@
   </si>
   <si>
     <t>13.05.2022</t>
+  </si>
+  <si>
+    <t>14.05.2022</t>
+  </si>
+  <si>
+    <t>Phd: Gumbel-Softmax Experiment Preparations</t>
+  </si>
+  <si>
+    <t>15.05.2022</t>
   </si>
 </sst>
 </file>
@@ -1728,7 +1737,7 @@
       <charset val="162"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1787,6 +1796,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFBDD7EE"/>
         <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -1855,7 +1876,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1903,6 +1924,13 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -2917,10 +2945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2919"/>
+  <dimension ref="A1:G2959"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2898" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2909" sqref="D2909"/>
+    <sheetView tabSelected="1" topLeftCell="A2940" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2955" sqref="D2955"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37142,6 +37170,478 @@
         <v>4</v>
       </c>
       <c r="D2919" s="8"/>
+    </row>
+    <row r="2920" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2920" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="B2920" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2920" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2920" s="2"/>
+    </row>
+    <row r="2921" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2921" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2921" s="8">
+        <v>8</v>
+      </c>
+      <c r="C2921" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2921" s="10"/>
+    </row>
+    <row r="2922" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2922" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2922" s="8">
+        <v>24</v>
+      </c>
+      <c r="C2922" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2922" s="8"/>
+    </row>
+    <row r="2923" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2923" s="31" t="s">
+        <v>367</v>
+      </c>
+      <c r="B2923" s="31">
+        <v>4</v>
+      </c>
+      <c r="C2923" s="31">
+        <v>7</v>
+      </c>
+      <c r="D2923" s="8"/>
+    </row>
+    <row r="2924" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2924" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B2924" s="8">
+        <v>12</v>
+      </c>
+      <c r="C2924" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2924" s="8"/>
+    </row>
+    <row r="2925" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2925" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="B2925" s="8">
+        <v>6</v>
+      </c>
+      <c r="C2925" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2925" s="8"/>
+    </row>
+    <row r="2926" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2926" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="B2926" s="8">
+        <v>4</v>
+      </c>
+      <c r="C2926" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2926" s="8"/>
+    </row>
+    <row r="2927" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2927" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B2927" s="8">
+        <v>6</v>
+      </c>
+      <c r="C2927" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2927" s="8"/>
+    </row>
+    <row r="2928" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2928" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B2928" s="8">
+        <v>24</v>
+      </c>
+      <c r="C2928" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2928" s="8"/>
+    </row>
+    <row r="2929" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2929" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="B2929" s="8">
+        <v>12</v>
+      </c>
+      <c r="C2929" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2929" s="8"/>
+    </row>
+    <row r="2930" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2930" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="B2930" s="8">
+        <v>4</v>
+      </c>
+      <c r="C2930" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2930" s="8"/>
+    </row>
+    <row r="2931" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2931" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="B2931" s="8">
+        <v>6</v>
+      </c>
+      <c r="C2931" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2931" s="8"/>
+    </row>
+    <row r="2932" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2932" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="B2932" s="8">
+        <v>3</v>
+      </c>
+      <c r="C2932" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2932" s="8"/>
+    </row>
+    <row r="2933" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2933" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="B2933" s="8">
+        <v>24</v>
+      </c>
+      <c r="C2933" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2933" s="8"/>
+    </row>
+    <row r="2934" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2934" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="B2934" s="8">
+        <v>24</v>
+      </c>
+      <c r="C2934" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2934" s="8"/>
+    </row>
+    <row r="2935" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2935" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="B2935" s="8">
+        <v>10</v>
+      </c>
+      <c r="C2935" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2935" s="8"/>
+    </row>
+    <row r="2936" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2936" s="32" t="s">
+        <v>550</v>
+      </c>
+      <c r="B2936" s="32">
+        <v>6</v>
+      </c>
+      <c r="C2936" s="32">
+        <v>3</v>
+      </c>
+      <c r="D2936" s="8"/>
+    </row>
+    <row r="2937" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2937" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="B2937" s="8">
+        <v>6</v>
+      </c>
+      <c r="C2937" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2937" s="8"/>
+    </row>
+    <row r="2938" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2938" s="19" t="s">
+        <v>468</v>
+      </c>
+      <c r="B2938" s="19">
+        <v>8</v>
+      </c>
+      <c r="C2938" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2939" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2939" s="8"/>
+      <c r="B2939" s="8">
+        <f>SUM(B2921:B2938)</f>
+        <v>191</v>
+      </c>
+      <c r="C2939" s="8">
+        <f>SUM(C2921:C2938)</f>
+        <v>10</v>
+      </c>
+      <c r="D2939" s="8"/>
+    </row>
+    <row r="2940" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2940" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B2940" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2940" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2940" s="2"/>
+    </row>
+    <row r="2941" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2941" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2941" s="8">
+        <v>8</v>
+      </c>
+      <c r="C2941" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2941" s="33"/>
+    </row>
+    <row r="2942" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2942" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2942" s="8">
+        <v>24</v>
+      </c>
+      <c r="C2942" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2942" s="34"/>
+    </row>
+    <row r="2943" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2943" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B2943" s="8">
+        <v>12</v>
+      </c>
+      <c r="C2943" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2943" s="34"/>
+    </row>
+    <row r="2944" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2944" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="B2944" s="8">
+        <v>6</v>
+      </c>
+      <c r="C2944" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2944" s="34"/>
+    </row>
+    <row r="2945" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2945" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="B2945" s="8">
+        <v>4</v>
+      </c>
+      <c r="C2945" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2945" s="34"/>
+    </row>
+    <row r="2946" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2946" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B2946" s="8">
+        <v>6</v>
+      </c>
+      <c r="C2946" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2946" s="34"/>
+    </row>
+    <row r="2947" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2947" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B2947" s="8">
+        <v>24</v>
+      </c>
+      <c r="C2947" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2947" s="34"/>
+    </row>
+    <row r="2948" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2948" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="B2948" s="8">
+        <v>12</v>
+      </c>
+      <c r="C2948" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2948" s="34"/>
+    </row>
+    <row r="2949" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2949" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="B2949" s="8">
+        <v>4</v>
+      </c>
+      <c r="C2949" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2949" s="34"/>
+    </row>
+    <row r="2950" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2950" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="B2950" s="8">
+        <v>6</v>
+      </c>
+      <c r="C2950" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2950" s="34"/>
+    </row>
+    <row r="2951" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2951" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="B2951" s="8">
+        <v>3</v>
+      </c>
+      <c r="C2951" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2951" s="34"/>
+    </row>
+    <row r="2952" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2952" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="B2952" s="8">
+        <v>24</v>
+      </c>
+      <c r="C2952" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2952" s="34"/>
+    </row>
+    <row r="2953" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2953" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="B2953" s="8">
+        <v>24</v>
+      </c>
+      <c r="C2953" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2953" s="34"/>
+    </row>
+    <row r="2954" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2954" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="B2954" s="8">
+        <v>10</v>
+      </c>
+      <c r="C2954" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2954" s="34"/>
+    </row>
+    <row r="2955" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2955" s="32" t="s">
+        <v>550</v>
+      </c>
+      <c r="B2955" s="32">
+        <v>6</v>
+      </c>
+      <c r="C2955" s="8">
+        <v>3</v>
+      </c>
+      <c r="D2955" s="34"/>
+    </row>
+    <row r="2956" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2956" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="B2956" s="8">
+        <v>6</v>
+      </c>
+      <c r="C2956" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2956" s="34"/>
+    </row>
+    <row r="2957" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2957" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="B2957" s="8">
+        <v>8</v>
+      </c>
+      <c r="C2957" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2957" s="34"/>
+    </row>
+    <row r="2958" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2958" s="35"/>
+      <c r="B2958" s="35"/>
+      <c r="C2958" s="35"/>
+    </row>
+    <row r="2959" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2959" s="8"/>
+      <c r="B2959" s="8">
+        <f>SUM(B2941:B2957)</f>
+        <v>187</v>
+      </c>
+      <c r="C2959" s="8">
+        <f>SUM(C2941:C2957)</f>
+        <v>3</v>
+      </c>
+      <c r="D2959" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Straight Through option added.
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\phd_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00F0B5D-0019-433E-B216-08F37554DF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0476C4-85F8-4163-98FC-C8ED66468F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3300" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3301" uniqueCount="553">
   <si>
     <t>ToDo</t>
   </si>
@@ -1701,6 +1701,9 @@
   </si>
   <si>
     <t>15.05.2022</t>
+  </si>
+  <si>
+    <t>Phd: Gumbel-Softmax Straight Through Implementation</t>
   </si>
 </sst>
 </file>
@@ -2948,7 +2951,7 @@
   <dimension ref="A1:G2959"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2940" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2955" sqref="D2955"/>
+      <selection activeCell="C2958" sqref="C2958"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37598,7 +37601,7 @@
         <v>6</v>
       </c>
       <c r="C2955" s="8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2955" s="34"/>
     </row>
@@ -37627,19 +37630,25 @@
       <c r="D2957" s="34"/>
     </row>
     <row r="2958" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2958" s="35"/>
-      <c r="B2958" s="35"/>
-      <c r="C2958" s="35"/>
+      <c r="A2958" s="35" t="s">
+        <v>552</v>
+      </c>
+      <c r="B2958" s="35">
+        <v>4</v>
+      </c>
+      <c r="C2958" s="35">
+        <v>0</v>
+      </c>
     </row>
     <row r="2959" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2959" s="8"/>
       <c r="B2959" s="8">
-        <f>SUM(B2941:B2957)</f>
-        <v>187</v>
+        <f>SUM(B2941:B2958)</f>
+        <v>191</v>
       </c>
       <c r="C2959" s="8">
-        <f>SUM(C2941:C2957)</f>
-        <v>3</v>
+        <f>SUM(C2941:C2958)</f>
+        <v>6</v>
       </c>
       <c r="D2959" s="34"/>
     </row>

</xml_diff>

<commit_message>
Gumbel Softmax looks better now: Use softmax for decision activation nonlinearity and use Straight Through Estimator.
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3345" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3367" uniqueCount="561">
   <si>
     <t xml:space="preserve">ToDo</t>
   </si>
@@ -1471,16 +1471,16 @@
     <t xml:space="preserve">Phd: Start paperspace experiments</t>
   </si>
   <si>
+    <t xml:space="preserve">Phd: Test single path routing potential of CIGTs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blackshark: OSM Data preparation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phd: Start new experiments</t>
+  </si>
+  <si>
     <t xml:space="preserve">18.05.2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phd: Test single path routing potential of CIGTs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blackshark: OSM Data preparation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phd: Start new experiments</t>
   </si>
   <si>
     <t xml:space="preserve">MNIST</t>
@@ -1912,7 +1912,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2045,8 +2045,20 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2122,7 +2134,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2406,11 +2418,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="87910223"/>
-        <c:axId val="86568964"/>
+        <c:axId val="7718945"/>
+        <c:axId val="43656809"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87910223"/>
+        <c:axId val="7718945"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2452,12 +2464,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86568964"/>
+        <c:crossAx val="43656809"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86568964"/>
+        <c:axId val="43656809"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2499,7 +2511,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87910223"/>
+        <c:crossAx val="7718945"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2558,13 +2570,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1546</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>303840</xdr:colOff>
       <xdr:row>1547</xdr:row>
-      <xdr:rowOff>120960</xdr:rowOff>
+      <xdr:rowOff>121320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2573,7 +2585,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9691920" y="283120920"/>
+          <a:off x="9691920" y="283121280"/>
           <a:ext cx="303840" cy="303840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2598,13 +2610,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1558</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>303840</xdr:colOff>
       <xdr:row>1559</xdr:row>
-      <xdr:rowOff>120960</xdr:rowOff>
+      <xdr:rowOff>121320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2613,7 +2625,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9691920" y="285864120"/>
+          <a:off x="9691920" y="285864480"/>
           <a:ext cx="303840" cy="303840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2676,10 +2688,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3001"/>
+  <dimension ref="A1:G3022"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2975" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2996" activeCellId="0" sqref="D2996"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2996" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3020" activeCellId="0" sqref="D3020"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -37612,7 +37624,7 @@
     </row>
     <row r="2981" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2981" s="1" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B2981" s="2" t="s">
         <v>0</v>
@@ -37777,18 +37789,18 @@
     </row>
     <row r="2996" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2996" s="8" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B2996" s="8" t="n">
         <v>5</v>
       </c>
       <c r="C2996" s="8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2997" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2997" s="8" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B2997" s="8" t="n">
         <v>8</v>
@@ -37821,13 +37833,13 @@
     </row>
     <row r="3000" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3000" s="8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B3000" s="8" t="n">
         <v>2</v>
       </c>
       <c r="C3000" s="8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3001" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37837,7 +37849,237 @@
       </c>
       <c r="C3001" s="8" t="n">
         <f aca="false">SUM(C2982:C3000)</f>
-        <v>6</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3002" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3002" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B3002" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3002" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3003" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3003" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B3003" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3003" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3004" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3004" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3004" s="8" t="n">
+        <v>24</v>
+      </c>
+      <c r="C3004" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3005" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3005" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3005" s="8" t="n">
+        <v>12</v>
+      </c>
+      <c r="C3005" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3006" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3006" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="B3006" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C3006" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3007" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3007" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="B3007" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3007" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3008" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3008" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B3008" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C3008" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3009" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3009" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B3009" s="8" t="n">
+        <v>24</v>
+      </c>
+      <c r="C3009" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3010" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3010" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="B3010" s="8" t="n">
+        <v>12</v>
+      </c>
+      <c r="C3010" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3011" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3011" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="B3011" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3011" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3012" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3012" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="B3012" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C3012" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3013" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3013" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="B3013" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3013" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3014" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3014" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="B3014" s="8" t="n">
+        <v>24</v>
+      </c>
+      <c r="C3014" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3015" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3015" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="B3015" s="8" t="n">
+        <v>24</v>
+      </c>
+      <c r="C3015" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3016" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3016" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="B3016" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3016" s="8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3017" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3017" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="B3017" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3017" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3018" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3018" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="B3018" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3018" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3019" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3019" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="B3019" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3019" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3020" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3020" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="B3020" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3020" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3021" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3021" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="B3021" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3021" s="8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3022" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3022" s="8" t="n">
+        <f aca="false">SUM(B3003:B3021)</f>
+        <v>192</v>
+      </c>
+      <c r="C3022" s="8" t="n">
+        <f aca="false">SUM(C3003:C3021)</f>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -40133,10 +40375,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -40162,7 +40404,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="33" t="s">
         <v>538</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -40170,15 +40412,15 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>539</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="33" t="n">
         <v>388</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="33" t="s">
         <v>540</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -40186,7 +40428,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="33" t="s">
         <v>541</v>
       </c>
       <c r="B6" s="0" t="n">
@@ -40194,7 +40436,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="33" t="s">
         <v>542</v>
       </c>
       <c r="B7" s="0" t="n">
@@ -40202,7 +40444,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="33" t="s">
         <v>543</v>
       </c>
       <c r="B8" s="0" t="n">
@@ -40210,7 +40452,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="33" t="s">
         <v>544</v>
       </c>
       <c r="B9" s="0" t="n">
@@ -40218,7 +40460,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="33" t="s">
         <v>545</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -40226,7 +40468,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="33" t="s">
         <v>546</v>
       </c>
       <c r="B11" s="0" t="n">
@@ -40234,7 +40476,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="33" t="s">
         <v>547</v>
       </c>
       <c r="B12" s="0" t="n">
@@ -40242,7 +40484,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="33" t="s">
         <v>548</v>
       </c>
       <c r="B13" s="0" t="n">
@@ -40250,15 +40492,15 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="33" t="s">
         <v>549</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="35" t="s">
         <v>550</v>
       </c>
       <c r="B15" s="0" t="n">
@@ -40266,15 +40508,15 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="33" t="s">
         <v>551</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="36" t="s">
         <v>552</v>
       </c>
       <c r="B17" s="0" t="n">
@@ -40282,7 +40524,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="33" t="s">
         <v>552</v>
       </c>
       <c r="B18" s="0" t="n">
@@ -40290,7 +40532,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="33" t="s">
         <v>553</v>
       </c>
       <c r="B19" s="0" t="n">
@@ -40316,7 +40558,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="33" t="s">
         <v>557</v>
       </c>
       <c r="B23" s="0" t="n">
@@ -40324,7 +40566,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="33" t="s">
         <v>557</v>
       </c>
       <c r="B24" s="0" t="n">
@@ -40332,7 +40574,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="33" t="s">
         <v>557</v>
       </c>
       <c r="B25" s="0" t="n">
@@ -40340,7 +40582,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="33" t="s">
         <v>557</v>
       </c>
       <c r="B26" s="0" t="n">
@@ -40348,7 +40590,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="33" t="s">
         <v>558</v>
       </c>
       <c r="B27" s="0" t="n">
@@ -40356,7 +40598,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="33" t="s">
         <v>559</v>
       </c>
       <c r="B28" s="0" t="n">
@@ -40377,6 +40619,61 @@
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="n">
         <v>189</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D36" s="0" t="n">
+        <v>0.92330002784729</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D37" s="0" t="n">
+        <v>0.922599971294403</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D38" s="0" t="n">
+        <v>0.923099994659424</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D39" s="0" t="n">
+        <v>0.923200011253357</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D40" s="0" t="n">
+        <v>0.922900021076202</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D41" s="0" t="n">
+        <v>0.922699987888336</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D42" s="0" t="n">
+        <v>0.923099994659424</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D43" s="0" t="n">
+        <v>0.922699987888336</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D44" s="0" t="n">
+        <v>0.922800004482269</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D45" s="0" t="n">
+        <v>0.922100007534027</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D46" s="0" t="n">
+        <v>0.923699975013733</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Launched experiments on TETAM and TETAM Tuna
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\phd_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A0C448-7D3E-407A-8342-05DD9610444A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47671FF5-FD29-4747-84FA-DA0C84068A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38825,7 +38825,7 @@
         <v>2</v>
       </c>
       <c r="C3061" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3062" spans="1:3">
@@ -38851,7 +38851,7 @@
       </c>
       <c r="C3064" s="8">
         <f>SUM(C3045:C3063)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Added small db for experiment queries. -Bayesian Optimization Class system for subclassing for every new set of experiment.
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\phd_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA804E4-925E-480F-9116-4DBE54E628F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D0BD29-792E-4CDB-A21F-53A5790CBB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3410" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3454" uniqueCount="576">
   <si>
     <t>ToDo</t>
   </si>
@@ -1752,6 +1752,27 @@
   </si>
   <si>
     <t>Blackshark: Read POC documents for height estimation</t>
+  </si>
+  <si>
+    <t>24.05.2022</t>
+  </si>
+  <si>
+    <t>Blackshark: Prepare World Grid</t>
+  </si>
+  <si>
+    <t>Blackshark: Setup PostGIS</t>
+  </si>
+  <si>
+    <t>Blackshark: Gather building vector data</t>
+  </si>
+  <si>
+    <t>Insumo: Gather productivity estimation features</t>
+  </si>
+  <si>
+    <t>25.05.2022</t>
+  </si>
+  <si>
+    <t>Blackshark: Docker localhost problem</t>
   </si>
 </sst>
 </file>
@@ -1794,7 +1815,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1873,6 +1894,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -1939,7 +1966,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1999,6 +2026,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -3013,10 +3041,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3064"/>
+  <dimension ref="A1:G3106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3041" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3052" sqref="D3052"/>
+    <sheetView tabSelected="1" topLeftCell="A3083" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3090" sqref="D3090"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
@@ -38810,7 +38838,7 @@
         <v>8</v>
       </c>
       <c r="C3059" s="8">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3060" spans="1:3">
@@ -38858,7 +38886,467 @@
       </c>
       <c r="C3064" s="8">
         <f>SUM(C3045:C3063)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3065" spans="1:3">
+      <c r="A3065" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B3065" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3065" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3066" spans="1:3">
+      <c r="A3066" s="37" t="s">
+        <v>573</v>
+      </c>
+      <c r="B3066" s="37">
+        <v>10</v>
+      </c>
+      <c r="C3066" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3067" spans="1:3">
+      <c r="A3067" s="37" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3067" s="37">
+        <v>24</v>
+      </c>
+      <c r="C3067" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3068" spans="1:3">
+      <c r="A3068" s="37" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3068" s="37">
+        <v>12</v>
+      </c>
+      <c r="C3068" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3069" spans="1:3">
+      <c r="A3069" s="37" t="s">
+        <v>439</v>
+      </c>
+      <c r="B3069" s="37">
+        <v>6</v>
+      </c>
+      <c r="C3069" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3070" spans="1:3">
+      <c r="A3070" s="37" t="s">
+        <v>426</v>
+      </c>
+      <c r="B3070" s="37">
+        <v>4</v>
+      </c>
+      <c r="C3070" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3071" spans="1:3">
+      <c r="A3071" s="37" t="s">
+        <v>400</v>
+      </c>
+      <c r="B3071" s="37">
+        <v>6</v>
+      </c>
+      <c r="C3071" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3072" spans="1:3">
+      <c r="A3072" s="37" t="s">
+        <v>404</v>
+      </c>
+      <c r="B3072" s="37">
+        <v>24</v>
+      </c>
+      <c r="C3072" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3073" spans="1:3">
+      <c r="A3073" s="37" t="s">
+        <v>405</v>
+      </c>
+      <c r="B3073" s="37">
+        <v>12</v>
+      </c>
+      <c r="C3073" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3074" spans="1:3">
+      <c r="A3074" s="37" t="s">
+        <v>408</v>
+      </c>
+      <c r="B3074" s="37">
+        <v>4</v>
+      </c>
+      <c r="C3074" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3075" spans="1:3">
+      <c r="A3075" s="37" t="s">
+        <v>566</v>
+      </c>
+      <c r="B3075" s="37">
         <v>3</v>
+      </c>
+      <c r="C3075" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3076" spans="1:3">
+      <c r="A3076" s="37" t="s">
+        <v>427</v>
+      </c>
+      <c r="B3076" s="37">
+        <v>3</v>
+      </c>
+      <c r="C3076" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3077" spans="1:3">
+      <c r="A3077" s="37" t="s">
+        <v>450</v>
+      </c>
+      <c r="B3077" s="37">
+        <v>24</v>
+      </c>
+      <c r="C3077" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3078" spans="1:3">
+      <c r="A3078" s="37" t="s">
+        <v>451</v>
+      </c>
+      <c r="B3078" s="37">
+        <v>24</v>
+      </c>
+      <c r="C3078" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3079" spans="1:3">
+      <c r="A3079" s="37" t="s">
+        <v>480</v>
+      </c>
+      <c r="B3079" s="37">
+        <v>5</v>
+      </c>
+      <c r="C3079" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3080" spans="1:3">
+      <c r="A3080" s="37" t="s">
+        <v>570</v>
+      </c>
+      <c r="B3080" s="37">
+        <v>4</v>
+      </c>
+      <c r="C3080" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3081" spans="1:3">
+      <c r="A3081" s="37" t="s">
+        <v>563</v>
+      </c>
+      <c r="B3081" s="37">
+        <v>4</v>
+      </c>
+      <c r="C3081" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3082" spans="1:3">
+      <c r="A3082" s="38" t="s">
+        <v>571</v>
+      </c>
+      <c r="B3082" s="38">
+        <v>4</v>
+      </c>
+      <c r="C3082" s="36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3083" spans="1:3">
+      <c r="A3083" s="39" t="s">
+        <v>568</v>
+      </c>
+      <c r="B3083" s="39">
+        <v>2</v>
+      </c>
+      <c r="C3083" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3084" spans="1:3">
+      <c r="A3084" s="37" t="s">
+        <v>572</v>
+      </c>
+      <c r="B3084" s="37">
+        <v>6</v>
+      </c>
+      <c r="C3084" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3085" spans="1:3">
+      <c r="B3085" s="8">
+        <f>SUM(B3066:B3084)</f>
+        <v>181</v>
+      </c>
+      <c r="C3085" s="8">
+        <f>SUM(C3066:C3084)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3086" spans="1:3">
+      <c r="A3086" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B3086" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3086" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3087" spans="1:3">
+      <c r="A3087" s="37" t="s">
+        <v>573</v>
+      </c>
+      <c r="B3087" s="37">
+        <v>10</v>
+      </c>
+      <c r="C3087" s="37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3088" spans="1:3">
+      <c r="A3088" s="37" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3088" s="37">
+        <v>24</v>
+      </c>
+      <c r="C3088" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3089" spans="1:3">
+      <c r="A3089" s="37" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3089" s="37">
+        <v>12</v>
+      </c>
+      <c r="C3089" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3090" spans="1:3">
+      <c r="A3090" s="37" t="s">
+        <v>439</v>
+      </c>
+      <c r="B3090" s="37">
+        <v>6</v>
+      </c>
+      <c r="C3090" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3091" spans="1:3">
+      <c r="A3091" s="37" t="s">
+        <v>426</v>
+      </c>
+      <c r="B3091" s="37">
+        <v>4</v>
+      </c>
+      <c r="C3091" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3092" spans="1:3">
+      <c r="A3092" s="37" t="s">
+        <v>400</v>
+      </c>
+      <c r="B3092" s="37">
+        <v>6</v>
+      </c>
+      <c r="C3092" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3093" spans="1:3">
+      <c r="A3093" s="37" t="s">
+        <v>404</v>
+      </c>
+      <c r="B3093" s="37">
+        <v>24</v>
+      </c>
+      <c r="C3093" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3094" spans="1:3">
+      <c r="A3094" s="37" t="s">
+        <v>405</v>
+      </c>
+      <c r="B3094" s="37">
+        <v>12</v>
+      </c>
+      <c r="C3094" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3095" spans="1:3">
+      <c r="A3095" s="37" t="s">
+        <v>408</v>
+      </c>
+      <c r="B3095" s="37">
+        <v>4</v>
+      </c>
+      <c r="C3095" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3096" spans="1:3">
+      <c r="A3096" s="37" t="s">
+        <v>566</v>
+      </c>
+      <c r="B3096" s="37">
+        <v>3</v>
+      </c>
+      <c r="C3096" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3097" spans="1:3">
+      <c r="A3097" s="37" t="s">
+        <v>427</v>
+      </c>
+      <c r="B3097" s="37">
+        <v>3</v>
+      </c>
+      <c r="C3097" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3098" spans="1:3">
+      <c r="A3098" s="37" t="s">
+        <v>450</v>
+      </c>
+      <c r="B3098" s="37">
+        <v>24</v>
+      </c>
+      <c r="C3098" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3099" spans="1:3">
+      <c r="A3099" s="37" t="s">
+        <v>451</v>
+      </c>
+      <c r="B3099" s="37">
+        <v>24</v>
+      </c>
+      <c r="C3099" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3100" spans="1:3">
+      <c r="A3100" s="37" t="s">
+        <v>480</v>
+      </c>
+      <c r="B3100" s="37">
+        <v>5</v>
+      </c>
+      <c r="C3100" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3101" spans="1:3">
+      <c r="A3101" s="37" t="s">
+        <v>570</v>
+      </c>
+      <c r="B3101" s="37">
+        <v>4</v>
+      </c>
+      <c r="C3101" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3102" spans="1:3">
+      <c r="A3102" s="37" t="s">
+        <v>563</v>
+      </c>
+      <c r="B3102" s="37">
+        <v>4</v>
+      </c>
+      <c r="C3102" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3103" spans="1:3">
+      <c r="A3103" s="39" t="s">
+        <v>575</v>
+      </c>
+      <c r="B3103" s="39">
+        <v>2</v>
+      </c>
+      <c r="C3103" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3104" spans="1:3">
+      <c r="A3104" s="39" t="s">
+        <v>568</v>
+      </c>
+      <c r="B3104" s="39">
+        <v>2</v>
+      </c>
+      <c r="C3104" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3105" spans="1:3">
+      <c r="A3105" s="37" t="s">
+        <v>572</v>
+      </c>
+      <c r="B3105" s="37">
+        <v>6</v>
+      </c>
+      <c r="C3105" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3106" spans="1:3">
+      <c r="B3106" s="8">
+        <f>SUM(B3087:B3105)</f>
+        <v>179</v>
+      </c>
+      <c r="C3106" s="8">
+        <f>SUM(C3087:C3105)</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Random Routing has been added.
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\phd_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B862BD73-D72D-4B75-82F9-A7D18C97AF68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3024EBE9-4E47-48DD-B92D-97410ED9CF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3477" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3500" uniqueCount="580">
   <si>
     <t>ToDo</t>
   </si>
@@ -1782,6 +1782,9 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>27.05.2022</t>
   </si>
 </sst>
 </file>
@@ -3051,10 +3054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3127"/>
+  <dimension ref="A1:G3148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3117" sqref="D3117"/>
+    <sheetView tabSelected="1" topLeftCell="A3125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3137" sqref="D3137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
@@ -39466,7 +39469,7 @@
         <v>4</v>
       </c>
       <c r="C3116" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3117" spans="1:3">
@@ -39477,7 +39480,7 @@
         <v>3</v>
       </c>
       <c r="C3117" s="37">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3118" spans="1:3">
@@ -39589,7 +39592,240 @@
       </c>
       <c r="C3127" s="8">
         <f>SUM(C3108:C3126)</f>
-        <v>4</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3128" spans="1:3">
+      <c r="A3128" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B3128" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3128" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3129" spans="1:3">
+      <c r="A3129" s="37" t="s">
+        <v>573</v>
+      </c>
+      <c r="B3129" s="37">
+        <v>10</v>
+      </c>
+      <c r="C3129" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3130" spans="1:3">
+      <c r="A3130" s="37" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3130" s="37">
+        <v>24</v>
+      </c>
+      <c r="C3130" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3131" spans="1:3">
+      <c r="A3131" s="37" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3131" s="37">
+        <v>12</v>
+      </c>
+      <c r="C3131" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3132" spans="1:3">
+      <c r="A3132" s="37" t="s">
+        <v>439</v>
+      </c>
+      <c r="B3132" s="37">
+        <v>6</v>
+      </c>
+      <c r="C3132" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3133" spans="1:3">
+      <c r="A3133" s="37" t="s">
+        <v>426</v>
+      </c>
+      <c r="B3133" s="37">
+        <v>4</v>
+      </c>
+      <c r="C3133" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3134" spans="1:3">
+      <c r="A3134" s="37" t="s">
+        <v>577</v>
+      </c>
+      <c r="B3134" s="37">
+        <v>2</v>
+      </c>
+      <c r="C3134" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3135" spans="1:3">
+      <c r="A3135" s="37" t="s">
+        <v>404</v>
+      </c>
+      <c r="B3135" s="37">
+        <v>24</v>
+      </c>
+      <c r="C3135" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3136" spans="1:3">
+      <c r="A3136" s="37" t="s">
+        <v>405</v>
+      </c>
+      <c r="B3136" s="37">
+        <v>12</v>
+      </c>
+      <c r="C3136" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3137" spans="1:3">
+      <c r="A3137" s="37" t="s">
+        <v>408</v>
+      </c>
+      <c r="B3137" s="37">
+        <v>2</v>
+      </c>
+      <c r="C3137" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3138" spans="1:3">
+      <c r="A3138" s="37" t="s">
+        <v>566</v>
+      </c>
+      <c r="B3138" s="37">
+        <v>3</v>
+      </c>
+      <c r="C3138" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3139" spans="1:3">
+      <c r="A3139" s="37" t="s">
+        <v>427</v>
+      </c>
+      <c r="B3139" s="37">
+        <v>3</v>
+      </c>
+      <c r="C3139" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3140" spans="1:3">
+      <c r="A3140" s="37" t="s">
+        <v>450</v>
+      </c>
+      <c r="B3140" s="37">
+        <v>24</v>
+      </c>
+      <c r="C3140" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3141" spans="1:3">
+      <c r="A3141" s="37" t="s">
+        <v>451</v>
+      </c>
+      <c r="B3141" s="37">
+        <v>24</v>
+      </c>
+      <c r="C3141" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3142" spans="1:3">
+      <c r="A3142" s="37" t="s">
+        <v>480</v>
+      </c>
+      <c r="B3142" s="37">
+        <v>5</v>
+      </c>
+      <c r="C3142" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3143" spans="1:3">
+      <c r="A3143" s="37" t="s">
+        <v>570</v>
+      </c>
+      <c r="B3143" s="37">
+        <v>4</v>
+      </c>
+      <c r="C3143" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3144" spans="1:3">
+      <c r="A3144" s="37" t="s">
+        <v>563</v>
+      </c>
+      <c r="B3144" s="37">
+        <v>4</v>
+      </c>
+      <c r="C3144" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3145" spans="1:3">
+      <c r="A3145" s="39" t="s">
+        <v>575</v>
+      </c>
+      <c r="B3145" s="39">
+        <v>2</v>
+      </c>
+      <c r="C3145" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3146" spans="1:3">
+      <c r="A3146" s="39" t="s">
+        <v>568</v>
+      </c>
+      <c r="B3146" s="39">
+        <v>2</v>
+      </c>
+      <c r="C3146" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3147" spans="1:3">
+      <c r="A3147" s="37" t="s">
+        <v>572</v>
+      </c>
+      <c r="B3147" s="37">
+        <v>6</v>
+      </c>
+      <c r="C3147" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3148" spans="1:3">
+      <c r="A3148" s="40" t="s">
+        <v>578</v>
+      </c>
+      <c r="B3148" s="8">
+        <f>SUM(B3129:B3147)</f>
+        <v>173</v>
+      </c>
+      <c r="C3148" s="8">
+        <f>SUM(C3129:C3147)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Multipath capacity has been tested. Looks good!
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\phd_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD0F682-D547-4CBC-96FC-8BC47770B133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9EC581-8C5C-4AC7-91DF-7CDFB1879306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4716" yWindow="3396" windowWidth="17280" windowHeight="8964" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3746" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3825" uniqueCount="611">
   <si>
     <t>ToDo</t>
   </si>
@@ -1854,6 +1854,30 @@
   </si>
   <si>
     <t>9.06.2022</t>
+  </si>
+  <si>
+    <t>Phd: Devise threshold searching algorithm for multipath inference in CIGTs</t>
+  </si>
+  <si>
+    <t>10.06.2022</t>
+  </si>
+  <si>
+    <t>Blackshark: Create height landmarks</t>
+  </si>
+  <si>
+    <t>11-12.06.2022</t>
+  </si>
+  <si>
+    <t>13.06.2022</t>
+  </si>
+  <si>
+    <t>Phd: Read Homeworks</t>
+  </si>
+  <si>
+    <t>Insumo: Rule based productivity score deployment</t>
+  </si>
+  <si>
+    <t>14.06.2022</t>
   </si>
 </sst>
 </file>
@@ -1903,7 +1927,7 @@
       <charset val="162"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1976,6 +2000,12 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -2042,7 +2072,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2106,6 +2136,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -3120,10 +3151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3393"/>
+  <dimension ref="A1:G3481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3377" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3388" sqref="A3388"/>
+    <sheetView tabSelected="1" topLeftCell="A3455" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3473" sqref="D3473"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
@@ -42347,13 +42378,13 @@
     </row>
     <row r="3377" spans="1:3">
       <c r="A3377" s="8" t="s">
-        <v>426</v>
+        <v>603</v>
       </c>
       <c r="B3377" s="8">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C3377" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3378" spans="1:3">
@@ -42423,14 +42454,14 @@
       </c>
     </row>
     <row r="3384" spans="1:3">
-      <c r="A3384" s="8" t="s">
+      <c r="A3384" s="39" t="s">
         <v>598</v>
       </c>
-      <c r="B3384" s="8">
+      <c r="B3384" s="39">
         <v>5</v>
       </c>
-      <c r="C3384" s="8">
-        <v>2</v>
+      <c r="C3384" s="39">
+        <v>3</v>
       </c>
     </row>
     <row r="3385" spans="1:3">
@@ -42441,7 +42472,7 @@
         <v>12</v>
       </c>
       <c r="C3385" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3386" spans="1:3">
@@ -42507,11 +42538,901 @@
       <c r="A3393" s="26"/>
       <c r="B3393" s="8">
         <f>SUM(B3373:B3389)</f>
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C3393" s="8">
         <f>SUM(C3373:C3389)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3394" spans="1:3">
+      <c r="A3394" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="B3394" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3394" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3395" spans="1:3">
+      <c r="A3395" s="8" t="s">
+        <v>593</v>
+      </c>
+      <c r="B3395" s="8">
+        <v>4</v>
+      </c>
+      <c r="C3395" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3396" spans="1:3">
+      <c r="A3396" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3396" s="8">
+        <v>24</v>
+      </c>
+      <c r="C3396" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3397" spans="1:3">
+      <c r="A3397" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3397" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3397" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3398" spans="1:3">
+      <c r="A3398" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="B3398" s="8">
+        <v>6</v>
+      </c>
+      <c r="C3398" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3399" spans="1:3">
+      <c r="A3399" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="B3399" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3399" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3400" spans="1:3">
+      <c r="A3400" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B3400" s="8">
+        <v>24</v>
+      </c>
+      <c r="C3400" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3401" spans="1:3">
+      <c r="A3401" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="B3401" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3401" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3402" spans="1:3">
+      <c r="A3402" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="B3402" s="8">
+        <v>3</v>
+      </c>
+      <c r="C3402" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3403" spans="1:3">
+      <c r="A3403" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="B3403" s="8">
+        <v>3</v>
+      </c>
+      <c r="C3403" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3404" spans="1:3">
+      <c r="A3404" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="B3404" s="8">
+        <v>24</v>
+      </c>
+      <c r="C3404" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3405" spans="1:3">
+      <c r="A3405" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="B3405" s="8">
+        <v>24</v>
+      </c>
+      <c r="C3405" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3406" spans="1:3">
+      <c r="A3406" s="8" t="s">
+        <v>605</v>
+      </c>
+      <c r="B3406" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3406" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3407" spans="1:3">
+      <c r="A3407" s="8" t="s">
+        <v>594</v>
+      </c>
+      <c r="B3407" s="8">
+        <v>4</v>
+      </c>
+      <c r="C3407" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3408" spans="1:3">
+      <c r="A3408" s="26" t="s">
+        <v>595</v>
+      </c>
+      <c r="B3408" s="26">
+        <v>6</v>
+      </c>
+      <c r="C3408" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3409" spans="1:3">
+      <c r="A3409" s="26" t="s">
+        <v>596</v>
+      </c>
+      <c r="B3409" s="26">
+        <v>6</v>
+      </c>
+      <c r="C3409" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3410" spans="1:3">
+      <c r="A3410" s="26" t="s">
+        <v>597</v>
+      </c>
+      <c r="B3410" s="26">
+        <v>6</v>
+      </c>
+      <c r="C3410" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3411" spans="1:3">
+      <c r="A3411" s="26"/>
+      <c r="B3411" s="26"/>
+      <c r="C3411" s="26"/>
+    </row>
+    <row r="3412" spans="1:3">
+      <c r="A3412" s="26"/>
+      <c r="B3412" s="26"/>
+      <c r="C3412" s="26"/>
+    </row>
+    <row r="3413" spans="1:3">
+      <c r="A3413" s="26"/>
+      <c r="B3413" s="26"/>
+      <c r="C3413" s="26"/>
+    </row>
+    <row r="3414" spans="1:3">
+      <c r="A3414" s="26"/>
+      <c r="B3414" s="26"/>
+      <c r="C3414" s="26"/>
+    </row>
+    <row r="3415" spans="1:3">
+      <c r="A3415" s="26"/>
+      <c r="B3415" s="8">
+        <f>SUM(B3395:B3410)</f>
+        <v>182</v>
+      </c>
+      <c r="C3415" s="8">
+        <f>SUM(C3395:C3410)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3416" spans="1:3">
+      <c r="A3416" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="B3416" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3416" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3417" spans="1:3">
+      <c r="A3417" s="8" t="s">
+        <v>593</v>
+      </c>
+      <c r="B3417" s="8">
+        <v>4</v>
+      </c>
+      <c r="C3417" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3418" spans="1:3">
+      <c r="A3418" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3418" s="8">
+        <v>24</v>
+      </c>
+      <c r="C3418" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3419" spans="1:3">
+      <c r="A3419" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3419" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3419" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3420" spans="1:3">
+      <c r="A3420" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="B3420" s="8">
+        <v>6</v>
+      </c>
+      <c r="C3420" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3421" spans="1:3">
+      <c r="A3421" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="B3421" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3421" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3422" spans="1:3">
+      <c r="A3422" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B3422" s="8">
+        <v>24</v>
+      </c>
+      <c r="C3422" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3423" spans="1:3">
+      <c r="A3423" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="B3423" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3423" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3424" spans="1:3">
+      <c r="A3424" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="B3424" s="8">
+        <v>3</v>
+      </c>
+      <c r="C3424" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3425" spans="1:3">
+      <c r="A3425" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="B3425" s="8">
+        <v>3</v>
+      </c>
+      <c r="C3425" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3426" spans="1:3">
+      <c r="A3426" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="B3426" s="8">
+        <v>24</v>
+      </c>
+      <c r="C3426" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3427" spans="1:3">
+      <c r="A3427" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="B3427" s="8">
+        <v>24</v>
+      </c>
+      <c r="C3427" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3428" spans="1:3">
+      <c r="A3428" s="8" t="s">
+        <v>605</v>
+      </c>
+      <c r="B3428" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3428" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3429" spans="1:3">
+      <c r="A3429" s="8" t="s">
+        <v>594</v>
+      </c>
+      <c r="B3429" s="8">
+        <v>4</v>
+      </c>
+      <c r="C3429" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3430" spans="1:3">
+      <c r="A3430" s="26" t="s">
+        <v>595</v>
+      </c>
+      <c r="B3430" s="26">
+        <v>6</v>
+      </c>
+      <c r="C3430" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3431" spans="1:3">
+      <c r="A3431" s="26" t="s">
+        <v>596</v>
+      </c>
+      <c r="B3431" s="26">
+        <v>6</v>
+      </c>
+      <c r="C3431" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3432" spans="1:3">
+      <c r="A3432" s="26" t="s">
+        <v>597</v>
+      </c>
+      <c r="B3432" s="26">
+        <v>6</v>
+      </c>
+      <c r="C3432" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3433" spans="1:3">
+      <c r="A3433" s="26"/>
+      <c r="B3433" s="26"/>
+      <c r="C3433" s="26"/>
+    </row>
+    <row r="3434" spans="1:3">
+      <c r="A3434" s="26"/>
+      <c r="B3434" s="26"/>
+      <c r="C3434" s="26"/>
+    </row>
+    <row r="3435" spans="1:3">
+      <c r="A3435" s="26"/>
+      <c r="B3435" s="26"/>
+      <c r="C3435" s="26"/>
+    </row>
+    <row r="3436" spans="1:3">
+      <c r="A3436" s="26"/>
+      <c r="B3436" s="26"/>
+      <c r="C3436" s="26"/>
+    </row>
+    <row r="3437" spans="1:3">
+      <c r="A3437" s="26"/>
+      <c r="B3437" s="8">
+        <f>SUM(B3417:B3432)</f>
+        <v>182</v>
+      </c>
+      <c r="C3437" s="8">
+        <f>SUM(C3417:C3432)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3438" spans="1:3">
+      <c r="A3438" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="B3438" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3438" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3439" spans="1:3">
+      <c r="A3439" s="8" t="s">
+        <v>593</v>
+      </c>
+      <c r="B3439" s="8">
+        <v>4</v>
+      </c>
+      <c r="C3439" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3440" spans="1:3">
+      <c r="A3440" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3440" s="8">
+        <v>24</v>
+      </c>
+      <c r="C3440" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3441" spans="1:3">
+      <c r="A3441" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3441" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3441" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3442" spans="1:3">
+      <c r="A3442" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="B3442" s="8">
+        <v>6</v>
+      </c>
+      <c r="C3442" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3443" spans="1:3">
+      <c r="A3443" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="B3443" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3443" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3444" spans="1:3">
+      <c r="A3444" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B3444" s="8">
+        <v>24</v>
+      </c>
+      <c r="C3444" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3445" spans="1:3">
+      <c r="A3445" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="B3445" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3445" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3446" spans="1:3">
+      <c r="A3446" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="B3446" s="8">
+        <v>3</v>
+      </c>
+      <c r="C3446" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3447" spans="1:3">
+      <c r="A3447" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="B3447" s="8">
+        <v>3</v>
+      </c>
+      <c r="C3447" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3448" spans="1:3">
+      <c r="A3448" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="B3448" s="8">
+        <v>24</v>
+      </c>
+      <c r="C3448" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3449" spans="1:3">
+      <c r="A3449" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="B3449" s="8">
+        <v>24</v>
+      </c>
+      <c r="C3449" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3450" spans="1:3">
+      <c r="A3450" s="8" t="s">
+        <v>605</v>
+      </c>
+      <c r="B3450" s="8">
+        <v>4</v>
+      </c>
+      <c r="C3450" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3451" spans="1:3">
+      <c r="A3451" s="8" t="s">
+        <v>594</v>
+      </c>
+      <c r="B3451" s="8">
+        <v>4</v>
+      </c>
+      <c r="C3451" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3452" spans="1:3">
+      <c r="A3452" s="26" t="s">
+        <v>595</v>
+      </c>
+      <c r="B3452" s="26">
+        <v>6</v>
+      </c>
+      <c r="C3452" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3453" spans="1:3">
+      <c r="A3453" s="26" t="s">
+        <v>596</v>
+      </c>
+      <c r="B3453" s="26">
+        <v>6</v>
+      </c>
+      <c r="C3453" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3454" spans="1:3">
+      <c r="A3454" s="26" t="s">
+        <v>597</v>
+      </c>
+      <c r="B3454" s="26">
+        <v>6</v>
+      </c>
+      <c r="C3454" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3455" spans="1:3">
+      <c r="A3455" s="41" t="s">
+        <v>608</v>
+      </c>
+      <c r="B3455" s="41">
         <v>2</v>
+      </c>
+      <c r="C3455" s="41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3456" spans="1:3">
+      <c r="A3456" s="26" t="s">
+        <v>609</v>
+      </c>
+      <c r="B3456" s="26">
+        <v>3</v>
+      </c>
+      <c r="C3456" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3457" spans="1:3">
+      <c r="A3457" s="26"/>
+      <c r="B3457" s="26"/>
+      <c r="C3457" s="26"/>
+    </row>
+    <row r="3458" spans="1:3">
+      <c r="A3458" s="26"/>
+      <c r="B3458" s="26"/>
+      <c r="C3458" s="26"/>
+    </row>
+    <row r="3459" spans="1:3">
+      <c r="A3459" s="26"/>
+      <c r="B3459" s="8">
+        <f>SUM(B3439:B3456)</f>
+        <v>179</v>
+      </c>
+      <c r="C3459" s="8">
+        <f>SUM(C3439:C3456)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3460" spans="1:3">
+      <c r="A3460" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="B3460" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3460" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3461" spans="1:3">
+      <c r="A3461" s="8" t="s">
+        <v>593</v>
+      </c>
+      <c r="B3461" s="8">
+        <v>4</v>
+      </c>
+      <c r="C3461" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3462" spans="1:3">
+      <c r="A3462" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3462" s="8">
+        <v>24</v>
+      </c>
+      <c r="C3462" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3463" spans="1:3">
+      <c r="A3463" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3463" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3463" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3464" spans="1:3">
+      <c r="A3464" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="B3464" s="8">
+        <v>6</v>
+      </c>
+      <c r="C3464" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3465" spans="1:3">
+      <c r="A3465" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="B3465" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3465" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3466" spans="1:3">
+      <c r="A3466" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B3466" s="8">
+        <v>24</v>
+      </c>
+      <c r="C3466" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3467" spans="1:3">
+      <c r="A3467" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="B3467" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3467" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3468" spans="1:3">
+      <c r="A3468" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="B3468" s="8">
+        <v>3</v>
+      </c>
+      <c r="C3468" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3469" spans="1:3">
+      <c r="A3469" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="B3469" s="8">
+        <v>3</v>
+      </c>
+      <c r="C3469" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3470" spans="1:3">
+      <c r="A3470" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="B3470" s="8">
+        <v>24</v>
+      </c>
+      <c r="C3470" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3471" spans="1:3">
+      <c r="A3471" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="B3471" s="8">
+        <v>24</v>
+      </c>
+      <c r="C3471" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3472" spans="1:3">
+      <c r="A3472" s="8" t="s">
+        <v>605</v>
+      </c>
+      <c r="B3472" s="8">
+        <v>4</v>
+      </c>
+      <c r="C3472" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3473" spans="1:3">
+      <c r="A3473" s="8" t="s">
+        <v>594</v>
+      </c>
+      <c r="B3473" s="8">
+        <v>4</v>
+      </c>
+      <c r="C3473" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3474" spans="1:3">
+      <c r="A3474" s="26" t="s">
+        <v>595</v>
+      </c>
+      <c r="B3474" s="26">
+        <v>6</v>
+      </c>
+      <c r="C3474" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3475" spans="1:3">
+      <c r="A3475" s="26" t="s">
+        <v>596</v>
+      </c>
+      <c r="B3475" s="26">
+        <v>6</v>
+      </c>
+      <c r="C3475" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3476" spans="1:3">
+      <c r="A3476" s="26" t="s">
+        <v>597</v>
+      </c>
+      <c r="B3476" s="26">
+        <v>6</v>
+      </c>
+      <c r="C3476" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3477" spans="1:3">
+      <c r="A3477" s="26" t="s">
+        <v>609</v>
+      </c>
+      <c r="B3477" s="26">
+        <v>3</v>
+      </c>
+      <c r="C3477" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3478" spans="1:3">
+      <c r="A3478" s="26"/>
+      <c r="B3478" s="26"/>
+      <c r="C3478" s="26"/>
+    </row>
+    <row r="3479" spans="1:3">
+      <c r="A3479" s="26"/>
+      <c r="B3479" s="26"/>
+      <c r="C3479" s="26"/>
+    </row>
+    <row r="3480" spans="1:3">
+      <c r="A3480" s="26"/>
+      <c r="B3480" s="26"/>
+      <c r="C3480" s="26"/>
+    </row>
+    <row r="3481" spans="1:3">
+      <c r="A3481" s="26"/>
+      <c r="B3481" s="8">
+        <f>SUM(B3461:B3478)</f>
+        <v>177</v>
+      </c>
+      <c r="C3481" s="8">
+        <f>SUM(C3461:C3478)</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Entropies according to level decisions have been calculated.
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -2420,7 +2420,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2704,11 +2704,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="63447067"/>
-        <c:axId val="45638594"/>
+        <c:axId val="64743869"/>
+        <c:axId val="54002845"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63447067"/>
+        <c:axId val="64743869"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2750,12 +2750,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45638594"/>
+        <c:crossAx val="54002845"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45638594"/>
+        <c:axId val="54002845"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2797,7 +2797,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63447067"/>
+        <c:crossAx val="64743869"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2977,7 +2977,7 @@
   <dimension ref="A1:G3878"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3854" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3867" activeCellId="0" sqref="D3867"/>
+      <selection pane="topLeft" activeCell="D3863" activeCellId="0" sqref="D3863"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -47227,7 +47227,7 @@
         <v>6</v>
       </c>
       <c r="C3862" s="8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3863" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47379,7 +47379,7 @@
       </c>
       <c r="C3878" s="8" t="n">
         <f aca="false">SUM(C3858:C3875)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correctness and Mac calculations ready.
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -2423,7 +2423,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2707,11 +2707,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="84583532"/>
-        <c:axId val="5578804"/>
+        <c:axId val="84595823"/>
+        <c:axId val="85538079"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84583532"/>
+        <c:axId val="84595823"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2753,12 +2753,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5578804"/>
+        <c:crossAx val="85538079"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="5578804"/>
+        <c:axId val="85538079"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2800,7 +2800,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84583532"/>
+        <c:crossAx val="84595823"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2980,7 +2980,7 @@
   <dimension ref="A1:G3900"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3873" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3882" activeCellId="0" sqref="D3882"/>
+      <selection pane="topLeft" activeCell="D3888" activeCellId="0" sqref="D3888"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -47466,7 +47466,7 @@
         <v>6</v>
       </c>
       <c r="C3884" s="8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3885" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47624,7 +47624,7 @@
       </c>
       <c r="C3900" s="8" t="n">
         <f aca="false">SUM(C3880:C3898)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Probability Threshold Multipath Inference
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4440" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4463" uniqueCount="663">
   <si>
     <t xml:space="preserve">ToDo</t>
   </si>
@@ -1779,6 +1779,15 @@
   </si>
   <si>
     <t xml:space="preserve">19.07.2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.07.2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blackshark: Fix pretrained model loading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phd: Implement Probability Threshold based multiple path inference</t>
   </si>
   <si>
     <t xml:space="preserve">MNIST</t>
@@ -2478,7 +2487,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart79.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart93.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2762,11 +2771,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="67506788"/>
-        <c:axId val="98162149"/>
+        <c:axId val="15962858"/>
+        <c:axId val="38253093"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67506788"/>
+        <c:axId val="15962858"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2808,12 +2817,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98162149"/>
+        <c:crossAx val="38253093"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98162149"/>
+        <c:axId val="38253093"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2855,7 +2864,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67506788"/>
+        <c:crossAx val="15962858"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3032,10 +3041,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4124"/>
+  <dimension ref="A1:G4148"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4094" colorId="64" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4118" activeCellId="0" sqref="D4118"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4121" colorId="64" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4142" activeCellId="0" sqref="D4142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -50028,6 +50037,251 @@
       <c r="C4124" s="8" t="n">
         <f aca="false">SUM(C4102:C4123)</f>
         <v>4</v>
+      </c>
+    </row>
+    <row r="4125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4125" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B4125" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4125" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4126" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="B4126" s="8" t="n">
+        <v>24</v>
+      </c>
+      <c r="C4126" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4127" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B4127" s="8" t="n">
+        <v>12</v>
+      </c>
+      <c r="C4127" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4128" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="B4128" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4128" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4129" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B4129" s="8" t="n">
+        <v>24</v>
+      </c>
+      <c r="C4129" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4130" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="B4130" s="8" t="n">
+        <v>12</v>
+      </c>
+      <c r="C4130" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4131" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="B4131" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4131" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4132" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="B4132" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4132" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4133" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="B4133" s="8" t="n">
+        <v>24</v>
+      </c>
+      <c r="C4133" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4134" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="B4134" s="8" t="n">
+        <v>24</v>
+      </c>
+      <c r="C4134" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4135" s="8" t="s">
+        <v>518</v>
+      </c>
+      <c r="B4135" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4135" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4136" s="8" t="s">
+        <v>519</v>
+      </c>
+      <c r="B4136" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4136" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4137" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="B4137" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4137" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4138" s="8" t="s">
+        <v>541</v>
+      </c>
+      <c r="B4138" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4138" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4139" s="8" t="s">
+        <v>583</v>
+      </c>
+      <c r="B4139" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4139" s="8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4140" s="8" t="s">
+        <v>517</v>
+      </c>
+      <c r="B4140" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4140" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4141" s="8" t="s">
+        <v>573</v>
+      </c>
+      <c r="B4141" s="8" t="n">
+        <v>12</v>
+      </c>
+      <c r="C4141" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4142" s="8" t="s">
+        <v>574</v>
+      </c>
+      <c r="B4142" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4142" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4143" s="8" t="s">
+        <v>575</v>
+      </c>
+      <c r="B4143" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4143" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4144" s="8" t="s">
+        <v>577</v>
+      </c>
+      <c r="B4144" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4144" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4145" s="8" t="s">
+        <v>584</v>
+      </c>
+      <c r="B4145" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4145" s="8" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4146" s="8"/>
+    </row>
+    <row r="4147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4148" s="8" t="n">
+        <f aca="false">SUM(B4126:B4146)</f>
+        <v>187</v>
+      </c>
+      <c r="C4148" s="8" t="n">
+        <f aca="false">SUM(C4126:C4147)</f>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -50062,20 +50316,20 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50191,13 +50445,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50503,38 +50757,38 @@
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50545,7 +50799,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -50553,7 +50807,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H21" s="5" t="n">
         <v>80</v>
@@ -50567,7 +50821,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -50575,7 +50829,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H22" s="5" t="n">
         <v>80</v>
@@ -50589,7 +50843,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -50597,7 +50851,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H23" s="5" t="n">
         <v>80</v>
@@ -50611,17 +50865,17 @@
         <v>3</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H24" s="5" t="n">
         <v>80</v>
@@ -50635,17 +50889,17 @@
         <v>5</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H25" s="5" t="n">
         <v>80</v>
@@ -50659,17 +50913,17 @@
         <v>5</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H26" s="5" t="n">
         <v>80</v>
@@ -50683,17 +50937,17 @@
         <v>5</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H27" s="5" t="n">
         <v>80</v>
@@ -50707,17 +50961,17 @@
         <v>5</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H28" s="5" t="n">
         <v>80</v>
@@ -50731,17 +50985,17 @@
         <v>5</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="E29" s="32"/>
       <c r="F29" s="32" t="n">
         <v>0</v>
       </c>
       <c r="G29" s="32" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H29" s="32" t="n">
         <v>80</v>
@@ -50755,17 +51009,17 @@
         <v>5</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="E30" s="32"/>
       <c r="F30" s="32" t="n">
         <v>0</v>
       </c>
       <c r="G30" s="32" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H30" s="32" t="n">
         <v>80</v>
@@ -50779,17 +51033,17 @@
         <v>5</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="E31" s="32"/>
       <c r="F31" s="32" t="n">
         <v>0</v>
       </c>
       <c r="G31" s="32" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H31" s="32" t="n">
         <v>80</v>
@@ -50803,17 +51057,17 @@
         <v>5</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="E32" s="32"/>
       <c r="F32" s="32" t="n">
         <v>0</v>
       </c>
       <c r="G32" s="32" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H32" s="32" t="n">
         <v>80</v>
@@ -50827,17 +51081,17 @@
         <v>5</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="E33" s="32"/>
       <c r="F33" s="32" t="n">
         <v>0</v>
       </c>
       <c r="G33" s="32" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="H33" s="32" t="n">
         <v>80</v>
@@ -50851,17 +51105,17 @@
         <v>5</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="E34" s="32"/>
       <c r="F34" s="32" t="n">
         <v>0</v>
       </c>
       <c r="G34" s="32" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H34" s="32" t="n">
         <v>80</v>
@@ -50875,17 +51129,17 @@
         <v>5</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="D35" s="33" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="E35" s="33"/>
       <c r="F35" s="33" t="n">
         <v>0</v>
       </c>
       <c r="G35" s="33" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H35" s="33" t="n">
         <v>50</v>
@@ -50899,17 +51153,17 @@
         <v>5</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="D36" s="33" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="E36" s="33"/>
       <c r="F36" s="33" t="n">
         <v>0</v>
       </c>
       <c r="G36" s="33" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H36" s="33" t="n">
         <v>50</v>
@@ -50923,17 +51177,17 @@
         <v>5</v>
       </c>
       <c r="C37" s="33" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="E37" s="33"/>
       <c r="F37" s="33" t="n">
         <v>0</v>
       </c>
       <c r="G37" s="33" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H37" s="33" t="n">
         <v>50</v>
@@ -50947,20 +51201,20 @@
         <v>5</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="D38" s="33" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="E38" s="33"/>
       <c r="F38" s="33" t="n">
         <v>0</v>
       </c>
       <c r="G38" s="33" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="H38" s="33" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50980,22 +51234,22 @@
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D42" s="0" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D43" s="0" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D44" s="0" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D45" s="0" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52501,7 +52755,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B1" s="12" t="n">
         <v>329</v>
@@ -52509,7 +52763,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="39" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>379</v>
@@ -52517,7 +52771,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="39" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>399</v>
@@ -52525,7 +52779,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="40" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>388</v>
@@ -52533,7 +52787,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="39" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>50</v>
@@ -52541,7 +52795,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>9</v>
@@ -52549,7 +52803,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>11</v>
@@ -52557,7 +52811,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>3.5</v>
@@ -52565,7 +52819,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>7</v>
@@ -52573,7 +52827,7 @@
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>3</v>
@@ -52581,7 +52835,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>8</v>
@@ -52589,7 +52843,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>50</v>
@@ -52597,7 +52851,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>50</v>
@@ -52605,7 +52859,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>13</v>
@@ -52613,7 +52867,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>13</v>
@@ -52621,7 +52875,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>4</v>
@@ -52629,7 +52883,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>6.5</v>
@@ -52637,7 +52891,7 @@
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>6.5</v>
@@ -52645,7 +52899,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>7</v>
@@ -52653,17 +52907,17 @@
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>35</v>
@@ -52671,7 +52925,7 @@
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>6</v>
@@ -52679,7 +52933,7 @@
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>6</v>
@@ -52687,7 +52941,7 @@
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>6</v>
@@ -52695,7 +52949,7 @@
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>6</v>
@@ -52703,7 +52957,7 @@
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>15</v>
@@ -52711,7 +52965,7 @@
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>35</v>
@@ -52719,7 +52973,7 @@
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Sigmoid GMM distribution is implemented and tested.
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\phd_work2\phd_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC33B2A-F3FC-41B6-965E-7DA987FCDEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60EEC37-0D24-4479-969A-AB764381F3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5115" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5162" uniqueCount="738">
   <si>
     <t>ToDo</t>
   </si>
@@ -2227,13 +2227,46 @@
   </si>
   <si>
     <t>18.08.2022</t>
+  </si>
+  <si>
+    <t>19.08.2022</t>
+  </si>
+  <si>
+    <t>MT: Fix sql query</t>
+  </si>
+  <si>
+    <t>MT: Data downloader - MT: Fix sql query - product_images_table.download_status must be checked.</t>
+  </si>
+  <si>
+    <t>Phd: Sigmoid-GMM</t>
+  </si>
+  <si>
+    <t>Phd: Refactor CE Optimization, start experiments</t>
+  </si>
+  <si>
+    <t>MT: Analyze data statistics, get most common N classes.</t>
+  </si>
+  <si>
+    <t>MT: Model implementation in pytorch</t>
+  </si>
+  <si>
+    <t>Blackshark: Refactor Blackshark: Refactor datapreprocessing, pack it into a single class with a single table</t>
+  </si>
+  <si>
+    <t>MT: Flask image service</t>
+  </si>
+  <si>
+    <t>20-21.08.2022</t>
+  </si>
+  <si>
+    <t>Insumo: Create target variables for ML based productivity score estimation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2286,6 +2319,11 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2475,7 +2513,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2557,6 +2595,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -3571,10 +3611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4839"/>
+  <dimension ref="A1:G4892"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4813" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D4826" sqref="D4826"/>
+    <sheetView tabSelected="1" topLeftCell="A4867" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D4881" sqref="D4881"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -57840,7 +57880,7 @@
         <v>16</v>
       </c>
       <c r="C4828" s="26">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4829" spans="1:3">
@@ -57851,7 +57891,7 @@
         <v>6</v>
       </c>
       <c r="C4829" s="26">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4830" spans="1:3">
@@ -57899,14 +57939,14 @@
       </c>
     </row>
     <row r="4834" spans="1:3">
-      <c r="A4834" s="55" t="s">
+      <c r="A4834" s="54" t="s">
         <v>721</v>
       </c>
-      <c r="B4834" s="55">
+      <c r="B4834" s="54">
         <v>8</v>
       </c>
-      <c r="C4834" s="26">
-        <v>0</v>
+      <c r="C4834" s="54">
+        <v>5</v>
       </c>
     </row>
     <row r="4835" spans="1:3">
@@ -57937,7 +57977,528 @@
       </c>
       <c r="C4839" s="26">
         <f>SUM(C4814:C4838)</f>
-        <v>1</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4841" spans="1:3">
+      <c r="A4841" s="53" t="s">
+        <v>727</v>
+      </c>
+      <c r="B4841" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4841" s="53" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4842" spans="1:3">
+      <c r="A4842" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B4842" s="26">
+        <v>24</v>
+      </c>
+      <c r="C4842" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4843" spans="1:3">
+      <c r="A4843" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="B4843" s="26">
+        <v>12</v>
+      </c>
+      <c r="C4843" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4844" spans="1:3">
+      <c r="A4844" s="26" t="s">
+        <v>439</v>
+      </c>
+      <c r="B4844" s="26">
+        <v>6</v>
+      </c>
+      <c r="C4844" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4845" spans="1:3">
+      <c r="A4845" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="B4845" s="26">
+        <v>24</v>
+      </c>
+      <c r="C4845" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4846" spans="1:3">
+      <c r="A4846" s="26" t="s">
+        <v>405</v>
+      </c>
+      <c r="B4846" s="26">
+        <v>12</v>
+      </c>
+      <c r="C4846" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4847" spans="1:3">
+      <c r="A4847" s="26" t="s">
+        <v>487</v>
+      </c>
+      <c r="B4847" s="26">
+        <v>3</v>
+      </c>
+      <c r="C4847" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4848" spans="1:3">
+      <c r="A4848" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="B4848" s="26">
+        <v>3</v>
+      </c>
+      <c r="C4848" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4849" spans="1:3">
+      <c r="A4849" s="26" t="s">
+        <v>450</v>
+      </c>
+      <c r="B4849" s="26">
+        <v>24</v>
+      </c>
+      <c r="C4849" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4850" spans="1:3">
+      <c r="A4850" s="26" t="s">
+        <v>451</v>
+      </c>
+      <c r="B4850" s="26">
+        <v>24</v>
+      </c>
+      <c r="C4850" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4851" spans="1:3">
+      <c r="A4851" s="26" t="s">
+        <v>518</v>
+      </c>
+      <c r="B4851" s="26">
+        <v>6</v>
+      </c>
+      <c r="C4851" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4852" spans="1:3">
+      <c r="A4852" s="26" t="s">
+        <v>519</v>
+      </c>
+      <c r="B4852" s="26">
+        <v>2</v>
+      </c>
+      <c r="C4852" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4853" spans="1:3">
+      <c r="A4853" s="26" t="s">
+        <v>520</v>
+      </c>
+      <c r="B4853" s="26">
+        <v>6</v>
+      </c>
+      <c r="C4853" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4854" spans="1:3">
+      <c r="A4854" s="26" t="s">
+        <v>541</v>
+      </c>
+      <c r="B4854" s="26">
+        <v>2</v>
+      </c>
+      <c r="C4854" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4855" spans="1:3">
+      <c r="A4855" s="26" t="s">
+        <v>711</v>
+      </c>
+      <c r="B4855" s="26">
+        <v>2</v>
+      </c>
+      <c r="C4855" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4856" spans="1:3">
+      <c r="A4856" s="54" t="s">
+        <v>729</v>
+      </c>
+      <c r="B4856" s="54">
+        <v>16</v>
+      </c>
+      <c r="C4856" s="54">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4857" spans="1:3">
+      <c r="A4857" s="55" t="s">
+        <v>730</v>
+      </c>
+      <c r="B4857" s="55">
+        <v>12</v>
+      </c>
+      <c r="C4857" s="26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4858" spans="1:3">
+      <c r="A4858" s="54" t="s">
+        <v>709</v>
+      </c>
+      <c r="B4858" s="54">
+        <v>2</v>
+      </c>
+      <c r="C4858" s="54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4859" spans="1:3">
+      <c r="A4859" s="26" t="s">
+        <v>712</v>
+      </c>
+      <c r="B4859" s="26">
+        <v>6</v>
+      </c>
+      <c r="C4859" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4860" spans="1:3">
+      <c r="A4860" s="26" t="s">
+        <v>715</v>
+      </c>
+      <c r="B4860" s="26">
+        <v>12</v>
+      </c>
+      <c r="C4860" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4861" spans="1:3">
+      <c r="A4861" s="26" t="s">
+        <v>717</v>
+      </c>
+      <c r="B4861" s="26">
+        <v>4</v>
+      </c>
+      <c r="C4861" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4862" spans="1:3">
+      <c r="A4862" s="55" t="s">
+        <v>728</v>
+      </c>
+      <c r="B4862" s="55"/>
+      <c r="C4862" s="26"/>
+    </row>
+    <row r="4863" spans="1:3">
+      <c r="A4863" s="58"/>
+      <c r="B4863" s="58"/>
+      <c r="C4863" s="58"/>
+    </row>
+    <row r="4864" spans="1:3">
+      <c r="A4864" s="55"/>
+      <c r="B4864" s="55"/>
+      <c r="C4864" s="55"/>
+    </row>
+    <row r="4865" spans="1:3">
+      <c r="A4865" s="55"/>
+      <c r="B4865" s="55"/>
+      <c r="C4865" s="55"/>
+    </row>
+    <row r="4866" spans="1:3">
+      <c r="A4866" s="26"/>
+      <c r="B4866" s="26"/>
+      <c r="C4866" s="26"/>
+    </row>
+    <row r="4867" spans="1:3">
+      <c r="A4867" s="26"/>
+      <c r="B4867" s="26">
+        <f>SUM(B4842:B4866)</f>
+        <v>202</v>
+      </c>
+      <c r="C4867" s="26">
+        <f>SUM(C4842:C4866)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4869" spans="1:3">
+      <c r="A4869" s="53" t="s">
+        <v>736</v>
+      </c>
+      <c r="B4869" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4869" s="53" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4870" spans="1:3">
+      <c r="A4870" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B4870" s="26">
+        <v>24</v>
+      </c>
+      <c r="C4870" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4871" spans="1:3">
+      <c r="A4871" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="B4871" s="26">
+        <v>12</v>
+      </c>
+      <c r="C4871" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4872" spans="1:3">
+      <c r="A4872" s="26" t="s">
+        <v>439</v>
+      </c>
+      <c r="B4872" s="26">
+        <v>6</v>
+      </c>
+      <c r="C4872" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4873" spans="1:3">
+      <c r="A4873" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="B4873" s="26">
+        <v>24</v>
+      </c>
+      <c r="C4873" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4874" spans="1:3">
+      <c r="A4874" s="26" t="s">
+        <v>405</v>
+      </c>
+      <c r="B4874" s="26">
+        <v>12</v>
+      </c>
+      <c r="C4874" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4875" spans="1:3">
+      <c r="A4875" s="26" t="s">
+        <v>487</v>
+      </c>
+      <c r="B4875" s="26">
+        <v>3</v>
+      </c>
+      <c r="C4875" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4876" spans="1:3">
+      <c r="A4876" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="B4876" s="26">
+        <v>3</v>
+      </c>
+      <c r="C4876" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4877" spans="1:3">
+      <c r="A4877" s="26" t="s">
+        <v>450</v>
+      </c>
+      <c r="B4877" s="26">
+        <v>24</v>
+      </c>
+      <c r="C4877" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4878" spans="1:3">
+      <c r="A4878" s="60" t="s">
+        <v>451</v>
+      </c>
+      <c r="B4878" s="60">
+        <v>24</v>
+      </c>
+      <c r="C4878" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4879" spans="1:3">
+      <c r="A4879" s="60" t="s">
+        <v>541</v>
+      </c>
+      <c r="B4879" s="60">
+        <v>2</v>
+      </c>
+      <c r="C4879" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4880" spans="1:3">
+      <c r="A4880" s="60" t="s">
+        <v>711</v>
+      </c>
+      <c r="B4880" s="60">
+        <v>2</v>
+      </c>
+      <c r="C4880" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4881" spans="1:3">
+      <c r="A4881" s="60" t="s">
+        <v>732</v>
+      </c>
+      <c r="B4881" s="60">
+        <v>4</v>
+      </c>
+      <c r="C4881" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4882" spans="1:3">
+      <c r="A4882" s="59" t="s">
+        <v>730</v>
+      </c>
+      <c r="B4882" s="59">
+        <v>8</v>
+      </c>
+      <c r="C4882" s="60">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4883" spans="1:3">
+      <c r="A4883" s="60" t="s">
+        <v>737</v>
+      </c>
+      <c r="B4883" s="60">
+        <v>4</v>
+      </c>
+      <c r="C4883" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4884" spans="1:3">
+      <c r="A4884" s="60" t="s">
+        <v>715</v>
+      </c>
+      <c r="B4884" s="60">
+        <v>12</v>
+      </c>
+      <c r="C4884" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4885" spans="1:3">
+      <c r="A4885" s="60" t="s">
+        <v>717</v>
+      </c>
+      <c r="B4885" s="60">
+        <v>4</v>
+      </c>
+      <c r="C4885" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4886" spans="1:3">
+      <c r="A4886" s="60" t="s">
+        <v>731</v>
+      </c>
+      <c r="B4886" s="60">
+        <v>8</v>
+      </c>
+      <c r="C4886" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4887" spans="1:3">
+      <c r="A4887" s="59" t="s">
+        <v>733</v>
+      </c>
+      <c r="B4887" s="59">
+        <v>8</v>
+      </c>
+      <c r="C4887" s="60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4888" spans="1:3">
+      <c r="A4888" s="59" t="s">
+        <v>734</v>
+      </c>
+      <c r="B4888" s="59">
+        <v>6</v>
+      </c>
+      <c r="C4888" s="59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4889" spans="1:3">
+      <c r="A4889" s="59" t="s">
+        <v>735</v>
+      </c>
+      <c r="B4889" s="59">
+        <v>6</v>
+      </c>
+      <c r="C4889" s="59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4890" spans="1:3">
+      <c r="A4890" s="59"/>
+      <c r="B4890" s="59"/>
+      <c r="C4890" s="59"/>
+    </row>
+    <row r="4891" spans="1:3">
+      <c r="A4891" s="60"/>
+      <c r="B4891" s="60"/>
+      <c r="C4891" s="60"/>
+    </row>
+    <row r="4892" spans="1:3">
+      <c r="A4892" s="60"/>
+      <c r="B4892" s="60">
+        <f>SUM(B4870:B4891)</f>
+        <v>196</v>
+      </c>
+      <c r="C4892" s="60">
+        <f>SUM(C4870:C4891)</f>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring Cross Entropy Search based threshold optimization into a separate structure.
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\phd_work2\phd_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60EEC37-0D24-4479-969A-AB764381F3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54615EBE-9C2C-45D5-B1C9-47C538B2ACBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2513,7 +2513,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2595,6 +2595,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -3614,7 +3615,7 @@
   <dimension ref="A1:G4892"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4867" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D4881" sqref="D4881"/>
+      <selection activeCell="D4886" sqref="D4886"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -58349,46 +58350,46 @@
       </c>
     </row>
     <row r="4878" spans="1:3">
-      <c r="A4878" s="60" t="s">
+      <c r="A4878" s="61" t="s">
         <v>451</v>
       </c>
-      <c r="B4878" s="60">
+      <c r="B4878" s="61">
         <v>24</v>
       </c>
-      <c r="C4878" s="60">
+      <c r="C4878" s="61">
         <v>0</v>
       </c>
     </row>
     <row r="4879" spans="1:3">
-      <c r="A4879" s="60" t="s">
+      <c r="A4879" s="61" t="s">
         <v>541</v>
       </c>
-      <c r="B4879" s="60">
+      <c r="B4879" s="61">
         <v>2</v>
       </c>
-      <c r="C4879" s="60">
+      <c r="C4879" s="61">
         <v>0</v>
       </c>
     </row>
     <row r="4880" spans="1:3">
-      <c r="A4880" s="60" t="s">
+      <c r="A4880" s="61" t="s">
         <v>711</v>
       </c>
-      <c r="B4880" s="60">
+      <c r="B4880" s="61">
         <v>2</v>
       </c>
-      <c r="C4880" s="60">
+      <c r="C4880" s="61">
         <v>0</v>
       </c>
     </row>
     <row r="4881" spans="1:3">
-      <c r="A4881" s="60" t="s">
+      <c r="A4881" s="61" t="s">
         <v>732</v>
       </c>
-      <c r="B4881" s="60">
-        <v>4</v>
-      </c>
-      <c r="C4881" s="60">
+      <c r="B4881" s="61">
+        <v>4</v>
+      </c>
+      <c r="C4881" s="61">
         <v>0</v>
       </c>
     </row>
@@ -58399,106 +58400,106 @@
       <c r="B4882" s="59">
         <v>8</v>
       </c>
-      <c r="C4882" s="60">
+      <c r="C4882" s="59">
         <v>10</v>
       </c>
     </row>
     <row r="4883" spans="1:3">
-      <c r="A4883" s="60" t="s">
+      <c r="A4883" s="61" t="s">
         <v>737</v>
       </c>
-      <c r="B4883" s="60">
-        <v>4</v>
-      </c>
-      <c r="C4883" s="60">
+      <c r="B4883" s="61">
+        <v>4</v>
+      </c>
+      <c r="C4883" s="61">
         <v>0</v>
       </c>
     </row>
     <row r="4884" spans="1:3">
-      <c r="A4884" s="60" t="s">
+      <c r="A4884" s="61" t="s">
         <v>715</v>
       </c>
-      <c r="B4884" s="60">
+      <c r="B4884" s="61">
         <v>12</v>
       </c>
-      <c r="C4884" s="60">
+      <c r="C4884" s="61">
         <v>0</v>
       </c>
     </row>
     <row r="4885" spans="1:3">
-      <c r="A4885" s="60" t="s">
+      <c r="A4885" s="61" t="s">
         <v>717</v>
       </c>
-      <c r="B4885" s="60">
-        <v>4</v>
-      </c>
-      <c r="C4885" s="60">
+      <c r="B4885" s="61">
+        <v>4</v>
+      </c>
+      <c r="C4885" s="61">
         <v>0</v>
       </c>
     </row>
     <row r="4886" spans="1:3">
-      <c r="A4886" s="60" t="s">
+      <c r="A4886" s="61" t="s">
         <v>731</v>
       </c>
-      <c r="B4886" s="60">
+      <c r="B4886" s="61">
         <v>8</v>
       </c>
-      <c r="C4886" s="60">
-        <v>0</v>
+      <c r="C4886" s="61">
+        <v>2</v>
       </c>
     </row>
     <row r="4887" spans="1:3">
-      <c r="A4887" s="59" t="s">
+      <c r="A4887" s="60" t="s">
         <v>733</v>
       </c>
-      <c r="B4887" s="59">
+      <c r="B4887" s="60">
         <v>8</v>
       </c>
-      <c r="C4887" s="60">
+      <c r="C4887" s="61">
         <v>2</v>
       </c>
     </row>
     <row r="4888" spans="1:3">
-      <c r="A4888" s="59" t="s">
+      <c r="A4888" s="60" t="s">
         <v>734</v>
       </c>
-      <c r="B4888" s="59">
-        <v>6</v>
-      </c>
-      <c r="C4888" s="59">
+      <c r="B4888" s="60">
+        <v>6</v>
+      </c>
+      <c r="C4888" s="60">
         <v>0</v>
       </c>
     </row>
     <row r="4889" spans="1:3">
-      <c r="A4889" s="59" t="s">
+      <c r="A4889" s="60" t="s">
         <v>735</v>
       </c>
-      <c r="B4889" s="59">
-        <v>6</v>
-      </c>
-      <c r="C4889" s="59">
+      <c r="B4889" s="60">
+        <v>6</v>
+      </c>
+      <c r="C4889" s="60">
         <v>0</v>
       </c>
     </row>
     <row r="4890" spans="1:3">
-      <c r="A4890" s="59"/>
-      <c r="B4890" s="59"/>
-      <c r="C4890" s="59"/>
+      <c r="A4890" s="60"/>
+      <c r="B4890" s="60"/>
+      <c r="C4890" s="60"/>
     </row>
     <row r="4891" spans="1:3">
-      <c r="A4891" s="60"/>
-      <c r="B4891" s="60"/>
-      <c r="C4891" s="60"/>
+      <c r="A4891" s="61"/>
+      <c r="B4891" s="61"/>
+      <c r="C4891" s="61"/>
     </row>
     <row r="4892" spans="1:3">
-      <c r="A4892" s="60"/>
-      <c r="B4892" s="60">
+      <c r="A4892" s="61"/>
+      <c r="B4892" s="61">
         <f>SUM(B4870:B4891)</f>
         <v>196</v>
       </c>
-      <c r="C4892" s="60">
+      <c r="C4892" s="61">
         <f>SUM(C4870:C4891)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ready for Tetam experiments.
</commit_message>
<xml_diff>
--- a/Work Plan.xlsx
+++ b/Work Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\phd_work3\phd_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510AE4FF-D54A-4053-AF4F-CDE4D114F935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037B4E90-E5DF-4BFF-8087-A66020C10DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3682,8 +3682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5158" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D5174" sqref="D5174"/>
+    <sheetView tabSelected="1" topLeftCell="A5161" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B5173" sqref="B5173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -61493,7 +61493,7 @@
         <v>8</v>
       </c>
       <c r="C5175" s="5">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5176" spans="1:3">
@@ -61508,14 +61508,14 @@
       </c>
     </row>
     <row r="5177" spans="1:3">
-      <c r="A5177" s="53" t="s">
+      <c r="A5177" s="52" t="s">
         <v>750</v>
       </c>
-      <c r="B5177" s="53">
-        <v>6</v>
-      </c>
-      <c r="C5177" s="5">
-        <v>0</v>
+      <c r="B5177" s="52">
+        <v>6</v>
+      </c>
+      <c r="C5177" s="47">
+        <v>12</v>
       </c>
     </row>
     <row r="5178" spans="1:3">
@@ -61567,7 +61567,7 @@
       </c>
       <c r="C5183" s="53">
         <f>SUM(C5161:C5182)</f>
-        <v>8</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>